<commit_message>
Planned value in Progress
</commit_message>
<xml_diff>
--- a/13-ProgressReports/WP1-Prg.xlsx
+++ b/13-ProgressReports/WP1-Prg.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ken.long/KL-GIT/CCAP/02-LhARA/01-LhARA-costing-tool/13-ProgressReports/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35CD6DF9-7409-1543-B3F9-E97841DD4FA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{738C7C5C-A248-EA42-A966-8637D88F0D15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2600" yWindow="2700" windowWidth="27640" windowHeight="16940" xr2:uid="{CC2CDACD-23D9-2349-BC94-9046B71DD28A}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="WP1-Prg" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="22">
   <si>
     <t>Date:</t>
   </si>
@@ -85,12 +85,6 @@
     <t>Date</t>
   </si>
   <si>
-    <t>Planned % complete</t>
-  </si>
-  <si>
-    <t>% complete</t>
-  </si>
-  <si>
     <t>Spend</t>
   </si>
   <si>
@@ -103,7 +97,10 @@
     <t>ProgressLine</t>
   </si>
   <si>
-    <t>EndProgressRpt</t>
+    <t>Planned fraction complete</t>
+  </si>
+  <si>
+    <t>Fraction complete</t>
   </si>
 </sst>
 </file>
@@ -320,14 +317,14 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="9" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="3" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="3" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -644,8 +641,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B830DFFD-7C49-A743-A7AB-F5C942B0BCC3}">
   <dimension ref="A1:G70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="B36" sqref="B36"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -654,8 +651,8 @@
     <col min="2" max="2" width="59.6640625" customWidth="1"/>
     <col min="3" max="3" width="9.6640625" customWidth="1"/>
     <col min="4" max="4" width="19.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="26.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.5" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="13.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -727,32 +724,32 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B6" s="13" t="s">
         <v>11</v>
       </c>
       <c r="C6" s="25" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D6" s="19" t="s">
         <v>15</v>
       </c>
       <c r="E6" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="F6" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="G6" s="21" t="s">
         <v>16</v>
-      </c>
-      <c r="F6" s="20" t="s">
-        <v>17</v>
-      </c>
-      <c r="G6" s="21" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="B7" s="30" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" s="28" t="s">
         <v>12</v>
       </c>
       <c r="C7" s="26">
@@ -761,7 +758,7 @@
       <c r="D7" s="22">
         <v>44896</v>
       </c>
-      <c r="E7" s="28">
+      <c r="E7" s="30">
         <f>C7/60</f>
         <v>1.6666666666666666E-2</v>
       </c>
@@ -770,9 +767,9 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="B8" s="31" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" s="29" t="s">
         <v>12</v>
       </c>
       <c r="C8" s="27">
@@ -783,7 +780,7 @@
         <f>EDATE($D$7,C8)</f>
         <v>44958</v>
       </c>
-      <c r="E8" s="28">
+      <c r="E8" s="30">
         <f t="shared" ref="E8:E65" si="0">C8/60</f>
         <v>3.3333333333333333E-2</v>
       </c>
@@ -792,9 +789,9 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="B9" s="31" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" s="29" t="s">
         <v>12</v>
       </c>
       <c r="C9" s="27">
@@ -805,7 +802,7 @@
         <f t="shared" ref="D9:D65" si="2">EDATE($D$7,C9)</f>
         <v>44986</v>
       </c>
-      <c r="E9" s="28">
+      <c r="E9" s="30">
         <f t="shared" si="0"/>
         <v>0.05</v>
       </c>
@@ -814,9 +811,9 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="B10" s="31" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10" s="29" t="s">
         <v>12</v>
       </c>
       <c r="C10" s="27">
@@ -827,7 +824,7 @@
         <f t="shared" si="2"/>
         <v>45017</v>
       </c>
-      <c r="E10" s="28">
+      <c r="E10" s="30">
         <f t="shared" si="0"/>
         <v>6.6666666666666666E-2</v>
       </c>
@@ -836,9 +833,9 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="B11" s="31" t="s">
+        <v>19</v>
+      </c>
+      <c r="B11" s="29" t="s">
         <v>12</v>
       </c>
       <c r="C11" s="27">
@@ -849,7 +846,7 @@
         <f t="shared" si="2"/>
         <v>45047</v>
       </c>
-      <c r="E11" s="28">
+      <c r="E11" s="30">
         <f t="shared" si="0"/>
         <v>8.3333333333333329E-2</v>
       </c>
@@ -858,9 +855,9 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="B12" s="31" t="s">
+        <v>19</v>
+      </c>
+      <c r="B12" s="29" t="s">
         <v>12</v>
       </c>
       <c r="C12" s="27">
@@ -871,7 +868,7 @@
         <f t="shared" si="2"/>
         <v>45078</v>
       </c>
-      <c r="E12" s="28">
+      <c r="E12" s="30">
         <f t="shared" si="0"/>
         <v>0.1</v>
       </c>
@@ -880,9 +877,9 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="B13" s="31" t="s">
+        <v>19</v>
+      </c>
+      <c r="B13" s="29" t="s">
         <v>12</v>
       </c>
       <c r="C13" s="27">
@@ -893,7 +890,7 @@
         <f t="shared" si="2"/>
         <v>45108</v>
       </c>
-      <c r="E13" s="28">
+      <c r="E13" s="30">
         <f t="shared" si="0"/>
         <v>0.11666666666666667</v>
       </c>
@@ -902,9 +899,9 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="B14" s="31" t="s">
+        <v>19</v>
+      </c>
+      <c r="B14" s="29" t="s">
         <v>12</v>
       </c>
       <c r="C14" s="27">
@@ -915,7 +912,7 @@
         <f t="shared" si="2"/>
         <v>45139</v>
       </c>
-      <c r="E14" s="28">
+      <c r="E14" s="30">
         <f t="shared" si="0"/>
         <v>0.13333333333333333</v>
       </c>
@@ -924,9 +921,9 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="B15" s="31" t="s">
+        <v>19</v>
+      </c>
+      <c r="B15" s="29" t="s">
         <v>12</v>
       </c>
       <c r="C15" s="27">
@@ -937,7 +934,7 @@
         <f t="shared" si="2"/>
         <v>45170</v>
       </c>
-      <c r="E15" s="28">
+      <c r="E15" s="30">
         <f t="shared" si="0"/>
         <v>0.15</v>
       </c>
@@ -946,9 +943,9 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="B16" s="31" t="s">
+        <v>19</v>
+      </c>
+      <c r="B16" s="29" t="s">
         <v>12</v>
       </c>
       <c r="C16" s="27">
@@ -959,7 +956,7 @@
         <f t="shared" si="2"/>
         <v>45200</v>
       </c>
-      <c r="E16" s="28">
+      <c r="E16" s="30">
         <f t="shared" si="0"/>
         <v>0.16666666666666666</v>
       </c>
@@ -968,9 +965,9 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="B17" s="31" t="s">
+        <v>19</v>
+      </c>
+      <c r="B17" s="29" t="s">
         <v>12</v>
       </c>
       <c r="C17" s="27">
@@ -981,7 +978,7 @@
         <f t="shared" ref="D17:D49" si="3">EDATE($D$7,C17)</f>
         <v>45231</v>
       </c>
-      <c r="E17" s="28">
+      <c r="E17" s="30">
         <f t="shared" ref="E17:E49" si="4">C17/60</f>
         <v>0.18333333333333332</v>
       </c>
@@ -990,9 +987,9 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="B18" s="31" t="s">
+        <v>19</v>
+      </c>
+      <c r="B18" s="29" t="s">
         <v>12</v>
       </c>
       <c r="C18" s="27">
@@ -1003,7 +1000,7 @@
         <f t="shared" si="3"/>
         <v>45261</v>
       </c>
-      <c r="E18" s="28">
+      <c r="E18" s="30">
         <f t="shared" si="4"/>
         <v>0.2</v>
       </c>
@@ -1012,9 +1009,9 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="B19" s="31" t="s">
+        <v>19</v>
+      </c>
+      <c r="B19" s="29" t="s">
         <v>12</v>
       </c>
       <c r="C19" s="27">
@@ -1025,7 +1022,7 @@
         <f t="shared" si="3"/>
         <v>45292</v>
       </c>
-      <c r="E19" s="28">
+      <c r="E19" s="30">
         <f t="shared" si="4"/>
         <v>0.21666666666666667</v>
       </c>
@@ -1034,9 +1031,9 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="B20" s="31" t="s">
+        <v>19</v>
+      </c>
+      <c r="B20" s="29" t="s">
         <v>12</v>
       </c>
       <c r="C20" s="27">
@@ -1047,7 +1044,7 @@
         <f t="shared" si="3"/>
         <v>45323</v>
       </c>
-      <c r="E20" s="28">
+      <c r="E20" s="30">
         <f t="shared" si="4"/>
         <v>0.23333333333333334</v>
       </c>
@@ -1056,9 +1053,9 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="B21" s="31" t="s">
+        <v>19</v>
+      </c>
+      <c r="B21" s="29" t="s">
         <v>12</v>
       </c>
       <c r="C21" s="27">
@@ -1069,7 +1066,7 @@
         <f t="shared" si="3"/>
         <v>45352</v>
       </c>
-      <c r="E21" s="28">
+      <c r="E21" s="30">
         <f t="shared" si="4"/>
         <v>0.25</v>
       </c>
@@ -1078,9 +1075,9 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="B22" s="31" t="s">
+        <v>19</v>
+      </c>
+      <c r="B22" s="29" t="s">
         <v>12</v>
       </c>
       <c r="C22" s="27">
@@ -1091,7 +1088,7 @@
         <f t="shared" si="3"/>
         <v>45383</v>
       </c>
-      <c r="E22" s="28">
+      <c r="E22" s="30">
         <f t="shared" si="4"/>
         <v>0.26666666666666666</v>
       </c>
@@ -1100,9 +1097,9 @@
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="B23" s="31" t="s">
+        <v>19</v>
+      </c>
+      <c r="B23" s="29" t="s">
         <v>12</v>
       </c>
       <c r="C23" s="27">
@@ -1113,7 +1110,7 @@
         <f t="shared" si="3"/>
         <v>45413</v>
       </c>
-      <c r="E23" s="28">
+      <c r="E23" s="30">
         <f t="shared" si="4"/>
         <v>0.28333333333333333</v>
       </c>
@@ -1122,9 +1119,9 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="B24" s="31" t="s">
+        <v>19</v>
+      </c>
+      <c r="B24" s="29" t="s">
         <v>12</v>
       </c>
       <c r="C24" s="27">
@@ -1135,7 +1132,7 @@
         <f t="shared" si="3"/>
         <v>45444</v>
       </c>
-      <c r="E24" s="28">
+      <c r="E24" s="30">
         <f t="shared" si="4"/>
         <v>0.3</v>
       </c>
@@ -1144,9 +1141,9 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="B25" s="31" t="s">
+        <v>19</v>
+      </c>
+      <c r="B25" s="29" t="s">
         <v>12</v>
       </c>
       <c r="C25" s="27">
@@ -1157,7 +1154,7 @@
         <f t="shared" si="3"/>
         <v>45474</v>
       </c>
-      <c r="E25" s="28">
+      <c r="E25" s="30">
         <f t="shared" si="4"/>
         <v>0.31666666666666665</v>
       </c>
@@ -1166,9 +1163,9 @@
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="B26" s="31" t="s">
+        <v>19</v>
+      </c>
+      <c r="B26" s="29" t="s">
         <v>12</v>
       </c>
       <c r="C26" s="27">
@@ -1179,7 +1176,7 @@
         <f t="shared" si="3"/>
         <v>45505</v>
       </c>
-      <c r="E26" s="28">
+      <c r="E26" s="30">
         <f t="shared" si="4"/>
         <v>0.33333333333333331</v>
       </c>
@@ -1188,20 +1185,20 @@
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B27" s="29" t="s">
+        <v>12</v>
+      </c>
+      <c r="C27" s="27">
+        <f t="shared" si="1"/>
         <v>21</v>
       </c>
-      <c r="B27" s="31" t="s">
-        <v>12</v>
-      </c>
-      <c r="C27" s="27">
-        <f t="shared" si="1"/>
-        <v>21</v>
-      </c>
       <c r="D27" s="23">
         <f t="shared" si="3"/>
         <v>45536</v>
       </c>
-      <c r="E27" s="28">
+      <c r="E27" s="30">
         <f t="shared" si="4"/>
         <v>0.35</v>
       </c>
@@ -1210,9 +1207,9 @@
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="B28" s="31" t="s">
+        <v>19</v>
+      </c>
+      <c r="B28" s="29" t="s">
         <v>12</v>
       </c>
       <c r="C28" s="27">
@@ -1223,7 +1220,7 @@
         <f t="shared" si="3"/>
         <v>45566</v>
       </c>
-      <c r="E28" s="28">
+      <c r="E28" s="30">
         <f t="shared" si="4"/>
         <v>0.36666666666666664</v>
       </c>
@@ -1232,9 +1229,9 @@
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="B29" s="31" t="s">
+        <v>19</v>
+      </c>
+      <c r="B29" s="29" t="s">
         <v>12</v>
       </c>
       <c r="C29" s="27">
@@ -1245,7 +1242,7 @@
         <f t="shared" si="3"/>
         <v>45597</v>
       </c>
-      <c r="E29" s="28">
+      <c r="E29" s="30">
         <f t="shared" si="4"/>
         <v>0.38333333333333336</v>
       </c>
@@ -1254,9 +1251,9 @@
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="B30" s="31" t="s">
+        <v>19</v>
+      </c>
+      <c r="B30" s="29" t="s">
         <v>12</v>
       </c>
       <c r="C30" s="27">
@@ -1267,7 +1264,7 @@
         <f t="shared" si="3"/>
         <v>45627</v>
       </c>
-      <c r="E30" s="28">
+      <c r="E30" s="30">
         <f t="shared" si="4"/>
         <v>0.4</v>
       </c>
@@ -1276,9 +1273,9 @@
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="B31" s="31" t="s">
+        <v>19</v>
+      </c>
+      <c r="B31" s="29" t="s">
         <v>12</v>
       </c>
       <c r="C31" s="27">
@@ -1289,7 +1286,7 @@
         <f t="shared" si="3"/>
         <v>45658</v>
       </c>
-      <c r="E31" s="28">
+      <c r="E31" s="30">
         <f t="shared" si="4"/>
         <v>0.41666666666666669</v>
       </c>
@@ -1298,9 +1295,9 @@
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="B32" s="31" t="s">
+        <v>19</v>
+      </c>
+      <c r="B32" s="29" t="s">
         <v>12</v>
       </c>
       <c r="C32" s="27">
@@ -1311,7 +1308,7 @@
         <f t="shared" si="3"/>
         <v>45689</v>
       </c>
-      <c r="E32" s="28">
+      <c r="E32" s="30">
         <f t="shared" si="4"/>
         <v>0.43333333333333335</v>
       </c>
@@ -1320,9 +1317,9 @@
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A33" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="B33" s="31" t="s">
+        <v>19</v>
+      </c>
+      <c r="B33" s="29" t="s">
         <v>12</v>
       </c>
       <c r="C33" s="27">
@@ -1333,7 +1330,7 @@
         <f t="shared" si="3"/>
         <v>45717</v>
       </c>
-      <c r="E33" s="28">
+      <c r="E33" s="30">
         <f t="shared" si="4"/>
         <v>0.45</v>
       </c>
@@ -1342,9 +1339,9 @@
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A34" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="B34" s="31" t="s">
+        <v>19</v>
+      </c>
+      <c r="B34" s="29" t="s">
         <v>12</v>
       </c>
       <c r="C34" s="27">
@@ -1355,7 +1352,7 @@
         <f t="shared" si="3"/>
         <v>45748</v>
       </c>
-      <c r="E34" s="28">
+      <c r="E34" s="30">
         <f t="shared" si="4"/>
         <v>0.46666666666666667</v>
       </c>
@@ -1364,9 +1361,9 @@
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A35" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="B35" s="31" t="s">
+        <v>19</v>
+      </c>
+      <c r="B35" s="29" t="s">
         <v>12</v>
       </c>
       <c r="C35" s="27">
@@ -1377,7 +1374,7 @@
         <f t="shared" si="3"/>
         <v>45778</v>
       </c>
-      <c r="E35" s="28">
+      <c r="E35" s="30">
         <f t="shared" si="4"/>
         <v>0.48333333333333334</v>
       </c>
@@ -1386,9 +1383,9 @@
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A36" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="B36" s="31" t="s">
+        <v>19</v>
+      </c>
+      <c r="B36" s="29" t="s">
         <v>12</v>
       </c>
       <c r="C36" s="27">
@@ -1399,7 +1396,7 @@
         <f t="shared" si="3"/>
         <v>45809</v>
       </c>
-      <c r="E36" s="28">
+      <c r="E36" s="30">
         <f t="shared" si="4"/>
         <v>0.5</v>
       </c>
@@ -1408,9 +1405,9 @@
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A37" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="B37" s="31" t="s">
+        <v>19</v>
+      </c>
+      <c r="B37" s="29" t="s">
         <v>12</v>
       </c>
       <c r="C37" s="27">
@@ -1421,7 +1418,7 @@
         <f t="shared" si="3"/>
         <v>45839</v>
       </c>
-      <c r="E37" s="28">
+      <c r="E37" s="30">
         <f t="shared" si="4"/>
         <v>0.51666666666666672</v>
       </c>
@@ -1430,9 +1427,9 @@
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A38" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="B38" s="31" t="s">
+        <v>19</v>
+      </c>
+      <c r="B38" s="29" t="s">
         <v>12</v>
       </c>
       <c r="C38" s="27">
@@ -1443,7 +1440,7 @@
         <f t="shared" si="3"/>
         <v>45870</v>
       </c>
-      <c r="E38" s="28">
+      <c r="E38" s="30">
         <f t="shared" si="4"/>
         <v>0.53333333333333333</v>
       </c>
@@ -1452,9 +1449,9 @@
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A39" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="B39" s="31" t="s">
+        <v>19</v>
+      </c>
+      <c r="B39" s="29" t="s">
         <v>12</v>
       </c>
       <c r="C39" s="27">
@@ -1465,7 +1462,7 @@
         <f t="shared" si="3"/>
         <v>45901</v>
       </c>
-      <c r="E39" s="28">
+      <c r="E39" s="30">
         <f t="shared" si="4"/>
         <v>0.55000000000000004</v>
       </c>
@@ -1474,9 +1471,9 @@
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A40" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="B40" s="31" t="s">
+        <v>19</v>
+      </c>
+      <c r="B40" s="29" t="s">
         <v>12</v>
       </c>
       <c r="C40" s="27">
@@ -1487,7 +1484,7 @@
         <f t="shared" si="3"/>
         <v>45931</v>
       </c>
-      <c r="E40" s="28">
+      <c r="E40" s="30">
         <f t="shared" si="4"/>
         <v>0.56666666666666665</v>
       </c>
@@ -1496,9 +1493,9 @@
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A41" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="B41" s="31" t="s">
+        <v>19</v>
+      </c>
+      <c r="B41" s="29" t="s">
         <v>12</v>
       </c>
       <c r="C41" s="27">
@@ -1509,7 +1506,7 @@
         <f t="shared" si="3"/>
         <v>45962</v>
       </c>
-      <c r="E41" s="28">
+      <c r="E41" s="30">
         <f t="shared" si="4"/>
         <v>0.58333333333333337</v>
       </c>
@@ -1518,9 +1515,9 @@
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A42" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="B42" s="31" t="s">
+        <v>19</v>
+      </c>
+      <c r="B42" s="29" t="s">
         <v>12</v>
       </c>
       <c r="C42" s="27">
@@ -1531,7 +1528,7 @@
         <f t="shared" si="3"/>
         <v>45992</v>
       </c>
-      <c r="E42" s="28">
+      <c r="E42" s="30">
         <f t="shared" si="4"/>
         <v>0.6</v>
       </c>
@@ -1540,9 +1537,9 @@
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A43" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="B43" s="31" t="s">
+        <v>19</v>
+      </c>
+      <c r="B43" s="29" t="s">
         <v>12</v>
       </c>
       <c r="C43" s="27">
@@ -1553,7 +1550,7 @@
         <f t="shared" si="3"/>
         <v>46023</v>
       </c>
-      <c r="E43" s="28">
+      <c r="E43" s="30">
         <f t="shared" si="4"/>
         <v>0.6166666666666667</v>
       </c>
@@ -1562,9 +1559,9 @@
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A44" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="B44" s="31" t="s">
+        <v>19</v>
+      </c>
+      <c r="B44" s="29" t="s">
         <v>12</v>
       </c>
       <c r="C44" s="27">
@@ -1575,7 +1572,7 @@
         <f t="shared" si="3"/>
         <v>46054</v>
       </c>
-      <c r="E44" s="28">
+      <c r="E44" s="30">
         <f t="shared" si="4"/>
         <v>0.6333333333333333</v>
       </c>
@@ -1584,9 +1581,9 @@
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A45" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="B45" s="31" t="s">
+        <v>19</v>
+      </c>
+      <c r="B45" s="29" t="s">
         <v>12</v>
       </c>
       <c r="C45" s="27">
@@ -1597,7 +1594,7 @@
         <f t="shared" si="3"/>
         <v>46082</v>
       </c>
-      <c r="E45" s="28">
+      <c r="E45" s="30">
         <f t="shared" si="4"/>
         <v>0.65</v>
       </c>
@@ -1606,9 +1603,9 @@
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A46" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="B46" s="31" t="s">
+        <v>19</v>
+      </c>
+      <c r="B46" s="29" t="s">
         <v>12</v>
       </c>
       <c r="C46" s="27">
@@ -1619,7 +1616,7 @@
         <f t="shared" si="3"/>
         <v>46113</v>
       </c>
-      <c r="E46" s="28">
+      <c r="E46" s="30">
         <f t="shared" si="4"/>
         <v>0.66666666666666663</v>
       </c>
@@ -1628,9 +1625,9 @@
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A47" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="B47" s="31" t="s">
+        <v>19</v>
+      </c>
+      <c r="B47" s="29" t="s">
         <v>12</v>
       </c>
       <c r="C47" s="27">
@@ -1641,7 +1638,7 @@
         <f t="shared" si="3"/>
         <v>46143</v>
       </c>
-      <c r="E47" s="28">
+      <c r="E47" s="30">
         <f t="shared" si="4"/>
         <v>0.68333333333333335</v>
       </c>
@@ -1650,9 +1647,9 @@
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A48" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="B48" s="31" t="s">
+        <v>19</v>
+      </c>
+      <c r="B48" s="29" t="s">
         <v>12</v>
       </c>
       <c r="C48" s="27">
@@ -1663,7 +1660,7 @@
         <f t="shared" si="3"/>
         <v>46174</v>
       </c>
-      <c r="E48" s="28">
+      <c r="E48" s="30">
         <f t="shared" si="4"/>
         <v>0.7</v>
       </c>
@@ -1672,9 +1669,9 @@
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A49" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="B49" s="31" t="s">
+        <v>19</v>
+      </c>
+      <c r="B49" s="29" t="s">
         <v>12</v>
       </c>
       <c r="C49" s="27">
@@ -1685,7 +1682,7 @@
         <f t="shared" si="3"/>
         <v>46204</v>
       </c>
-      <c r="E49" s="28">
+      <c r="E49" s="30">
         <f t="shared" si="4"/>
         <v>0.71666666666666667</v>
       </c>
@@ -1694,9 +1691,9 @@
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A50" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="B50" s="31" t="s">
+        <v>19</v>
+      </c>
+      <c r="B50" s="29" t="s">
         <v>12</v>
       </c>
       <c r="C50" s="27">
@@ -1707,7 +1704,7 @@
         <f t="shared" si="2"/>
         <v>46235</v>
       </c>
-      <c r="E50" s="28">
+      <c r="E50" s="30">
         <f t="shared" si="0"/>
         <v>0.73333333333333328</v>
       </c>
@@ -1716,9 +1713,9 @@
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A51" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="B51" s="31" t="s">
+        <v>19</v>
+      </c>
+      <c r="B51" s="29" t="s">
         <v>12</v>
       </c>
       <c r="C51" s="27">
@@ -1729,7 +1726,7 @@
         <f t="shared" si="2"/>
         <v>46266</v>
       </c>
-      <c r="E51" s="28">
+      <c r="E51" s="30">
         <f t="shared" si="0"/>
         <v>0.75</v>
       </c>
@@ -1738,9 +1735,9 @@
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A52" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="B52" s="31" t="s">
+        <v>19</v>
+      </c>
+      <c r="B52" s="29" t="s">
         <v>12</v>
       </c>
       <c r="C52" s="27">
@@ -1751,7 +1748,7 @@
         <f t="shared" si="2"/>
         <v>46296</v>
       </c>
-      <c r="E52" s="28">
+      <c r="E52" s="30">
         <f t="shared" si="0"/>
         <v>0.76666666666666672</v>
       </c>
@@ -1760,9 +1757,9 @@
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A53" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="B53" s="31" t="s">
+        <v>19</v>
+      </c>
+      <c r="B53" s="29" t="s">
         <v>12</v>
       </c>
       <c r="C53" s="27">
@@ -1773,7 +1770,7 @@
         <f t="shared" si="2"/>
         <v>46327</v>
       </c>
-      <c r="E53" s="28">
+      <c r="E53" s="30">
         <f t="shared" si="0"/>
         <v>0.78333333333333333</v>
       </c>
@@ -1782,9 +1779,9 @@
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A54" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="B54" s="31" t="s">
+        <v>19</v>
+      </c>
+      <c r="B54" s="29" t="s">
         <v>12</v>
       </c>
       <c r="C54" s="27">
@@ -1795,7 +1792,7 @@
         <f t="shared" si="2"/>
         <v>46357</v>
       </c>
-      <c r="E54" s="28">
+      <c r="E54" s="30">
         <f t="shared" si="0"/>
         <v>0.8</v>
       </c>
@@ -1804,9 +1801,9 @@
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A55" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="B55" s="31" t="s">
+        <v>19</v>
+      </c>
+      <c r="B55" s="29" t="s">
         <v>12</v>
       </c>
       <c r="C55" s="27">
@@ -1817,7 +1814,7 @@
         <f t="shared" si="2"/>
         <v>46388</v>
       </c>
-      <c r="E55" s="28">
+      <c r="E55" s="30">
         <f t="shared" si="0"/>
         <v>0.81666666666666665</v>
       </c>
@@ -1826,9 +1823,9 @@
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A56" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="B56" s="31" t="s">
+        <v>19</v>
+      </c>
+      <c r="B56" s="29" t="s">
         <v>12</v>
       </c>
       <c r="C56" s="27">
@@ -1839,7 +1836,7 @@
         <f t="shared" si="2"/>
         <v>46419</v>
       </c>
-      <c r="E56" s="28">
+      <c r="E56" s="30">
         <f t="shared" si="0"/>
         <v>0.83333333333333337</v>
       </c>
@@ -1848,9 +1845,9 @@
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A57" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="B57" s="31" t="s">
+        <v>19</v>
+      </c>
+      <c r="B57" s="29" t="s">
         <v>12</v>
       </c>
       <c r="C57" s="27">
@@ -1861,7 +1858,7 @@
         <f t="shared" si="2"/>
         <v>46447</v>
       </c>
-      <c r="E57" s="28">
+      <c r="E57" s="30">
         <f t="shared" si="0"/>
         <v>0.85</v>
       </c>
@@ -1870,9 +1867,9 @@
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A58" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="B58" s="31" t="s">
+        <v>19</v>
+      </c>
+      <c r="B58" s="29" t="s">
         <v>12</v>
       </c>
       <c r="C58" s="27">
@@ -1883,7 +1880,7 @@
         <f t="shared" si="2"/>
         <v>46478</v>
       </c>
-      <c r="E58" s="28">
+      <c r="E58" s="30">
         <f t="shared" si="0"/>
         <v>0.8666666666666667</v>
       </c>
@@ -1892,9 +1889,9 @@
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A59" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="B59" s="31" t="s">
+        <v>19</v>
+      </c>
+      <c r="B59" s="29" t="s">
         <v>12</v>
       </c>
       <c r="C59" s="27">
@@ -1905,7 +1902,7 @@
         <f t="shared" si="2"/>
         <v>46508</v>
       </c>
-      <c r="E59" s="28">
+      <c r="E59" s="30">
         <f t="shared" si="0"/>
         <v>0.8833333333333333</v>
       </c>
@@ -1914,9 +1911,9 @@
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A60" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="B60" s="31" t="s">
+        <v>19</v>
+      </c>
+      <c r="B60" s="29" t="s">
         <v>12</v>
       </c>
       <c r="C60" s="27">
@@ -1927,7 +1924,7 @@
         <f t="shared" si="2"/>
         <v>46539</v>
       </c>
-      <c r="E60" s="28">
+      <c r="E60" s="30">
         <f t="shared" si="0"/>
         <v>0.9</v>
       </c>
@@ -1936,9 +1933,9 @@
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A61" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="B61" s="31" t="s">
+        <v>19</v>
+      </c>
+      <c r="B61" s="29" t="s">
         <v>12</v>
       </c>
       <c r="C61" s="27">
@@ -1949,7 +1946,7 @@
         <f t="shared" si="2"/>
         <v>46569</v>
       </c>
-      <c r="E61" s="28">
+      <c r="E61" s="30">
         <f t="shared" si="0"/>
         <v>0.91666666666666663</v>
       </c>
@@ -1958,9 +1955,9 @@
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A62" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="B62" s="31" t="s">
+        <v>19</v>
+      </c>
+      <c r="B62" s="29" t="s">
         <v>12</v>
       </c>
       <c r="C62" s="27">
@@ -1971,7 +1968,7 @@
         <f t="shared" si="2"/>
         <v>46600</v>
       </c>
-      <c r="E62" s="28">
+      <c r="E62" s="30">
         <f t="shared" si="0"/>
         <v>0.93333333333333335</v>
       </c>
@@ -1980,9 +1977,9 @@
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A63" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="B63" s="31" t="s">
+        <v>19</v>
+      </c>
+      <c r="B63" s="29" t="s">
         <v>12</v>
       </c>
       <c r="C63" s="27">
@@ -1993,7 +1990,7 @@
         <f t="shared" si="2"/>
         <v>46631</v>
       </c>
-      <c r="E63" s="28">
+      <c r="E63" s="30">
         <f t="shared" si="0"/>
         <v>0.95</v>
       </c>
@@ -2002,9 +1999,9 @@
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A64" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="B64" s="31" t="s">
+        <v>19</v>
+      </c>
+      <c r="B64" s="29" t="s">
         <v>12</v>
       </c>
       <c r="C64" s="27">
@@ -2015,7 +2012,7 @@
         <f t="shared" si="2"/>
         <v>46661</v>
       </c>
-      <c r="E64" s="28">
+      <c r="E64" s="30">
         <f t="shared" si="0"/>
         <v>0.96666666666666667</v>
       </c>
@@ -2024,9 +2021,9 @@
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A65" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="B65" s="31" t="s">
+        <v>19</v>
+      </c>
+      <c r="B65" s="29" t="s">
         <v>12</v>
       </c>
       <c r="C65" s="27">
@@ -2037,7 +2034,7 @@
         <f t="shared" si="2"/>
         <v>46692</v>
       </c>
-      <c r="E65" s="28">
+      <c r="E65" s="30">
         <f t="shared" si="0"/>
         <v>0.98333333333333328</v>
       </c>
@@ -2046,7 +2043,7 @@
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A66" s="5" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B66" s="16" t="s">
         <v>12</v>
@@ -2059,7 +2056,7 @@
         <f>EDATE($D$7,C66)</f>
         <v>46722</v>
       </c>
-      <c r="E66" s="29">
+      <c r="E66" s="31">
         <f>C66/60</f>
         <v>1</v>
       </c>

</xml_diff>

<commit_message>
Tidying post plot creation
</commit_message>
<xml_diff>
--- a/13-ProgressReports/WP1-Prg.xlsx
+++ b/13-ProgressReports/WP1-Prg.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ken.long/KL-GIT/CCAP/02-LhARA/01-LhARA-costing-tool/13-ProgressReports/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17500F3B-6D96-3444-9C83-9BA3D92B2626}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58D613D5-E436-BA4C-93DA-F46E5B800596}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2600" yWindow="640" windowWidth="27640" windowHeight="19000" xr2:uid="{CC2CDACD-23D9-2349-BC94-9046B71DD28A}"/>
   </bookViews>
@@ -592,8 +592,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B830DFFD-7C49-A743-A7AB-F5C942B0BCC3}">
   <dimension ref="A1:H70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="F28" sqref="F28"/>
+    <sheetView tabSelected="1" topLeftCell="A44" workbookViewId="0">
+      <selection activeCell="G66" sqref="G40:H66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -728,11 +728,11 @@
       </c>
       <c r="G7" s="27">
         <f ca="1">ABS(NORMINV(RAND(), E7, 2*1/60))</f>
-        <v>2.5733075649297804E-2</v>
+        <v>6.4372484581690675E-2</v>
       </c>
       <c r="H7" s="27">
         <f ca="1">G7*875</f>
-        <v>22.516441193135577</v>
+        <v>56.325924008979342</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
@@ -760,11 +760,11 @@
       </c>
       <c r="G8" s="27">
         <f t="shared" ref="G8:G65" ca="1" si="1">NORMINV(RAND(), E8, 2*1/60)</f>
-        <v>4.8229416718184238E-2</v>
+        <v>4.0642235576255833E-2</v>
       </c>
       <c r="H8" s="27">
         <f t="shared" ref="H8:H66" ca="1" si="2">G8*875</f>
-        <v>42.200739628411206</v>
+        <v>35.561956129223852</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
@@ -787,16 +787,16 @@
         <v>0.05</v>
       </c>
       <c r="F9" s="27">
-        <f t="shared" ref="F8:F66" si="5">E9*875</f>
+        <f t="shared" ref="F9:F66" si="5">E9*875</f>
         <v>43.75</v>
       </c>
       <c r="G9" s="27">
         <f t="shared" ca="1" si="1"/>
-        <v>1.2302757772623761E-2</v>
+        <v>7.676254684808767E-2</v>
       </c>
       <c r="H9" s="27">
         <f t="shared" ca="1" si="2"/>
-        <v>10.764913051045792</v>
+        <v>67.167228492076717</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
@@ -824,11 +824,11 @@
       </c>
       <c r="G10" s="27">
         <f t="shared" ca="1" si="1"/>
-        <v>7.9236599742196656E-2</v>
+        <v>9.8150185782451299E-2</v>
       </c>
       <c r="H10" s="27">
         <f t="shared" ca="1" si="2"/>
-        <v>69.332024774422081</v>
+        <v>85.881412559644886</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
@@ -856,11 +856,11 @@
       </c>
       <c r="G11" s="27">
         <f t="shared" ca="1" si="1"/>
-        <v>5.0500202758635586E-2</v>
+        <v>6.3919904682961992E-2</v>
       </c>
       <c r="H11" s="27">
         <f t="shared" ca="1" si="2"/>
-        <v>44.187677413806135</v>
+        <v>55.929916597591742</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
@@ -888,11 +888,11 @@
       </c>
       <c r="G12" s="27">
         <f t="shared" ca="1" si="1"/>
-        <v>0.12316662137289992</v>
+        <v>7.0573113622479977E-2</v>
       </c>
       <c r="H12" s="27">
         <f t="shared" ca="1" si="2"/>
-        <v>107.77079370128743</v>
+        <v>61.751474419669982</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
@@ -920,11 +920,11 @@
       </c>
       <c r="G13" s="27">
         <f t="shared" ca="1" si="1"/>
-        <v>9.822022495821775E-2</v>
+        <v>0.15414173062414083</v>
       </c>
       <c r="H13" s="27">
         <f t="shared" ca="1" si="2"/>
-        <v>85.942696838440526</v>
+        <v>134.87401429612322</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
@@ -952,11 +952,11 @@
       </c>
       <c r="G14" s="27">
         <f t="shared" ca="1" si="1"/>
-        <v>0.15447590322025012</v>
+        <v>0.1965677945742427</v>
       </c>
       <c r="H14" s="27">
         <f t="shared" ca="1" si="2"/>
-        <v>135.16641531771884</v>
+        <v>171.99682025246236</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
@@ -984,11 +984,11 @@
       </c>
       <c r="G15" s="27">
         <f t="shared" ca="1" si="1"/>
-        <v>0.15704994880771705</v>
+        <v>0.17255633445138713</v>
       </c>
       <c r="H15" s="27">
         <f t="shared" ca="1" si="2"/>
-        <v>137.41870520675243</v>
+        <v>150.98679264496374</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
@@ -1016,11 +1016,11 @@
       </c>
       <c r="G16" s="27">
         <f t="shared" ca="1" si="1"/>
-        <v>0.18705068720235496</v>
+        <v>0.18382697450407814</v>
       </c>
       <c r="H16" s="27">
         <f t="shared" ca="1" si="2"/>
-        <v>163.66935130206059</v>
+        <v>160.84860269106838</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.2">
@@ -1048,11 +1048,11 @@
       </c>
       <c r="G17" s="27">
         <f t="shared" ca="1" si="1"/>
-        <v>0.21130250852998642</v>
+        <v>0.16728110894099141</v>
       </c>
       <c r="H17" s="27">
         <f t="shared" ca="1" si="2"/>
-        <v>184.88969496373812</v>
+        <v>146.37097032336749</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.2">
@@ -1080,11 +1080,11 @@
       </c>
       <c r="G18" s="27">
         <f t="shared" ca="1" si="1"/>
-        <v>0.18440657297535784</v>
+        <v>0.12914501382021548</v>
       </c>
       <c r="H18" s="27">
         <f t="shared" ca="1" si="2"/>
-        <v>161.35575135343811</v>
+        <v>113.00188709268855</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.2">
@@ -1112,11 +1112,11 @@
       </c>
       <c r="G19" s="27">
         <f t="shared" ca="1" si="1"/>
-        <v>0.23110612182937737</v>
+        <v>0.20527339145965309</v>
       </c>
       <c r="H19" s="27">
         <f t="shared" ca="1" si="2"/>
-        <v>202.2178566007052</v>
+        <v>179.61421752719644</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.2">
@@ -1144,11 +1144,11 @@
       </c>
       <c r="G20" s="27">
         <f t="shared" ca="1" si="1"/>
-        <v>0.24759780924842345</v>
+        <v>0.30044899174154061</v>
       </c>
       <c r="H20" s="27">
         <f t="shared" ca="1" si="2"/>
-        <v>216.64808309237051</v>
+        <v>262.89286777384802</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.2">
@@ -1176,11 +1176,11 @@
       </c>
       <c r="G21" s="27">
         <f t="shared" ca="1" si="1"/>
-        <v>0.29165694972861805</v>
+        <v>0.30491094351252745</v>
       </c>
       <c r="H21" s="27">
         <f t="shared" ca="1" si="2"/>
-        <v>255.19983101254078</v>
+        <v>266.79707557346154</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.2">
@@ -1208,11 +1208,11 @@
       </c>
       <c r="G22" s="27">
         <f t="shared" ca="1" si="1"/>
-        <v>0.26188477434688234</v>
+        <v>0.24513354321508216</v>
       </c>
       <c r="H22" s="27">
         <f t="shared" ca="1" si="2"/>
-        <v>229.14917755352204</v>
+        <v>214.49185031319689</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.2">
@@ -1240,11 +1240,11 @@
       </c>
       <c r="G23" s="27">
         <f t="shared" ca="1" si="1"/>
-        <v>0.30523178213583946</v>
+        <v>0.24371360458226637</v>
       </c>
       <c r="H23" s="27">
         <f t="shared" ca="1" si="2"/>
-        <v>267.0778093688595</v>
+        <v>213.24940400948307</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.2">
@@ -1272,11 +1272,11 @@
       </c>
       <c r="G24" s="27">
         <f t="shared" ca="1" si="1"/>
-        <v>0.33654157123855077</v>
+        <v>0.26550359977237492</v>
       </c>
       <c r="H24" s="27">
         <f t="shared" ca="1" si="2"/>
-        <v>294.47387483373194</v>
+        <v>232.31564980082806</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.2">
@@ -1304,11 +1304,11 @@
       </c>
       <c r="G25" s="27">
         <f t="shared" ca="1" si="1"/>
-        <v>0.41879273677736828</v>
+        <v>0.30672510291308885</v>
       </c>
       <c r="H25" s="27">
         <f t="shared" ca="1" si="2"/>
-        <v>366.44364468019722</v>
+        <v>268.38446504895273</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.2">
@@ -1336,11 +1336,11 @@
       </c>
       <c r="G26" s="27">
         <f t="shared" ca="1" si="1"/>
-        <v>0.34178412000500313</v>
+        <v>0.31982558130285083</v>
       </c>
       <c r="H26" s="27">
         <f t="shared" ca="1" si="2"/>
-        <v>299.06110500437774</v>
+        <v>279.84738363999446</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.2">
@@ -1368,11 +1368,11 @@
       </c>
       <c r="G27" s="27">
         <f t="shared" ca="1" si="1"/>
-        <v>0.41028889721052142</v>
+        <v>0.37466583237197931</v>
       </c>
       <c r="H27" s="27">
         <f t="shared" ca="1" si="2"/>
-        <v>359.00278505920625</v>
+        <v>327.8326033254819</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.2">
@@ -1400,11 +1400,11 @@
       </c>
       <c r="G28" s="27">
         <f t="shared" ca="1" si="1"/>
-        <v>0.35249927827302224</v>
+        <v>0.35532524479600425</v>
       </c>
       <c r="H28" s="27">
         <f t="shared" ca="1" si="2"/>
-        <v>308.43686848889445</v>
+        <v>310.9095891965037</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.2">
@@ -1432,11 +1432,11 @@
       </c>
       <c r="G29" s="27">
         <f t="shared" ca="1" si="1"/>
-        <v>0.39056996865774546</v>
+        <v>0.38972730482226486</v>
       </c>
       <c r="H29" s="27">
         <f t="shared" ca="1" si="2"/>
-        <v>341.74872257552727</v>
+        <v>341.01139171948176</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.2">
@@ -1464,11 +1464,11 @@
       </c>
       <c r="G30" s="27">
         <f t="shared" ca="1" si="1"/>
-        <v>0.38101714602324604</v>
+        <v>0.39309279058344471</v>
       </c>
       <c r="H30" s="27">
         <f t="shared" ca="1" si="2"/>
-        <v>333.39000277034029</v>
+        <v>343.95619176051412</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.2">
@@ -1496,11 +1496,11 @@
       </c>
       <c r="G31" s="27">
         <f t="shared" ca="1" si="1"/>
-        <v>0.39178456467072509</v>
+        <v>0.41295511972014465</v>
       </c>
       <c r="H31" s="27">
         <f t="shared" ca="1" si="2"/>
-        <v>342.81149408688447</v>
+        <v>361.33572975512658</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.2">
@@ -1528,11 +1528,11 @@
       </c>
       <c r="G32" s="27">
         <f t="shared" ca="1" si="1"/>
-        <v>0.44308129592774714</v>
+        <v>0.44920441192154331</v>
       </c>
       <c r="H32" s="27">
         <f t="shared" ca="1" si="2"/>
-        <v>387.69613393677872</v>
+        <v>393.05386043135042</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.2">
@@ -1560,11 +1560,11 @@
       </c>
       <c r="G33" s="27">
         <f t="shared" ca="1" si="1"/>
-        <v>0.44293035923880925</v>
+        <v>0.45044818547739274</v>
       </c>
       <c r="H33" s="27">
         <f t="shared" ca="1" si="2"/>
-        <v>387.56406433395807</v>
+        <v>394.14216229271864</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.2">
@@ -1592,11 +1592,11 @@
       </c>
       <c r="G34" s="27">
         <f t="shared" ca="1" si="1"/>
-        <v>0.42055197158333757</v>
+        <v>0.50309377235679309</v>
       </c>
       <c r="H34" s="27">
         <f t="shared" ca="1" si="2"/>
-        <v>367.98297513542036</v>
+        <v>440.20705081219393</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.2">
@@ -1624,11 +1624,11 @@
       </c>
       <c r="G35" s="27">
         <f t="shared" ca="1" si="1"/>
-        <v>0.42888661826032265</v>
+        <v>0.49426154173244563</v>
       </c>
       <c r="H35" s="27">
         <f t="shared" ca="1" si="2"/>
-        <v>375.27579097778232</v>
+        <v>432.47884901588992</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.2">
@@ -1656,11 +1656,11 @@
       </c>
       <c r="G36" s="27">
         <f t="shared" ca="1" si="1"/>
-        <v>0.53989448370900195</v>
+        <v>0.50377584050539581</v>
       </c>
       <c r="H36" s="27">
         <f t="shared" ca="1" si="2"/>
-        <v>472.40767324537671</v>
+        <v>440.80386044222132</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.2">
@@ -1688,11 +1688,11 @@
       </c>
       <c r="G37" s="27">
         <f t="shared" ca="1" si="1"/>
-        <v>0.51701251730873432</v>
+        <v>0.53249337236775085</v>
       </c>
       <c r="H37" s="27">
         <f t="shared" ca="1" si="2"/>
-        <v>452.38595264514254</v>
+        <v>465.93170082178199</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.2">
@@ -1720,11 +1720,11 @@
       </c>
       <c r="G38" s="27">
         <f t="shared" ca="1" si="1"/>
-        <v>0.52110224311108622</v>
+        <v>0.53949929442053834</v>
       </c>
       <c r="H38" s="27">
         <f t="shared" ca="1" si="2"/>
-        <v>455.96446272220044</v>
+        <v>472.06188261797104</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.2">
@@ -1752,11 +1752,11 @@
       </c>
       <c r="G39" s="27">
         <f t="shared" ca="1" si="1"/>
-        <v>0.58234871085756135</v>
+        <v>0.59000217624986973</v>
       </c>
       <c r="H39" s="27">
         <f t="shared" ca="1" si="2"/>
-        <v>509.55512200036617</v>
+        <v>516.25190421863601</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.2">
@@ -1782,14 +1782,8 @@
         <f t="shared" si="5"/>
         <v>495.83333333333331</v>
       </c>
-      <c r="G40" s="27">
-        <f t="shared" ca="1" si="1"/>
-        <v>0.61637293306726582</v>
-      </c>
-      <c r="H40" s="27">
-        <f t="shared" ca="1" si="2"/>
-        <v>539.32631643385764</v>
-      </c>
+      <c r="G40" s="27"/>
+      <c r="H40" s="27"/>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A41" s="5" t="s">
@@ -1814,14 +1808,8 @@
         <f t="shared" si="5"/>
         <v>510.41666666666669</v>
       </c>
-      <c r="G41" s="27">
-        <f t="shared" ca="1" si="1"/>
-        <v>0.65756062482076616</v>
-      </c>
-      <c r="H41" s="27">
-        <f t="shared" ca="1" si="2"/>
-        <v>575.36554671817044</v>
-      </c>
+      <c r="G41" s="27"/>
+      <c r="H41" s="27"/>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A42" s="5" t="s">
@@ -1846,14 +1834,8 @@
         <f t="shared" si="5"/>
         <v>525</v>
       </c>
-      <c r="G42" s="27">
-        <f t="shared" ca="1" si="1"/>
-        <v>0.52754172486701056</v>
-      </c>
-      <c r="H42" s="27">
-        <f t="shared" ca="1" si="2"/>
-        <v>461.59900925863423</v>
-      </c>
+      <c r="G42" s="27"/>
+      <c r="H42" s="27"/>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A43" s="5" t="s">
@@ -1878,14 +1860,8 @@
         <f t="shared" si="5"/>
         <v>539.58333333333337</v>
       </c>
-      <c r="G43" s="27">
-        <f t="shared" ca="1" si="1"/>
-        <v>0.62080674881166131</v>
-      </c>
-      <c r="H43" s="27">
-        <f t="shared" ca="1" si="2"/>
-        <v>543.2059052102037</v>
-      </c>
+      <c r="G43" s="27"/>
+      <c r="H43" s="27"/>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A44" s="5" t="s">
@@ -1910,14 +1886,8 @@
         <f t="shared" si="5"/>
         <v>554.16666666666663</v>
       </c>
-      <c r="G44" s="27">
-        <f t="shared" ca="1" si="1"/>
-        <v>0.59520759372053766</v>
-      </c>
-      <c r="H44" s="27">
-        <f t="shared" ca="1" si="2"/>
-        <v>520.80664450547044</v>
-      </c>
+      <c r="G44" s="27"/>
+      <c r="H44" s="27"/>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A45" s="5" t="s">
@@ -1942,14 +1912,8 @@
         <f t="shared" si="5"/>
         <v>568.75</v>
       </c>
-      <c r="G45" s="27">
-        <f t="shared" ca="1" si="1"/>
-        <v>0.69575655859136842</v>
-      </c>
-      <c r="H45" s="27">
-        <f t="shared" ca="1" si="2"/>
-        <v>608.78698876744738</v>
-      </c>
+      <c r="G45" s="27"/>
+      <c r="H45" s="27"/>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A46" s="5" t="s">
@@ -1974,14 +1938,8 @@
         <f t="shared" si="5"/>
         <v>583.33333333333326</v>
       </c>
-      <c r="G46" s="27">
-        <f t="shared" ca="1" si="1"/>
-        <v>0.68021193152482806</v>
-      </c>
-      <c r="H46" s="27">
-        <f t="shared" ca="1" si="2"/>
-        <v>595.18544008422452</v>
-      </c>
+      <c r="G46" s="27"/>
+      <c r="H46" s="27"/>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A47" s="5" t="s">
@@ -2006,14 +1964,8 @@
         <f t="shared" si="5"/>
         <v>597.91666666666663</v>
       </c>
-      <c r="G47" s="27">
-        <f t="shared" ca="1" si="1"/>
-        <v>0.72523840220572677</v>
-      </c>
-      <c r="H47" s="27">
-        <f t="shared" ca="1" si="2"/>
-        <v>634.5836019300109</v>
-      </c>
+      <c r="G47" s="27"/>
+      <c r="H47" s="27"/>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A48" s="5" t="s">
@@ -2038,14 +1990,8 @@
         <f t="shared" si="5"/>
         <v>612.5</v>
       </c>
-      <c r="G48" s="27">
-        <f t="shared" ca="1" si="1"/>
-        <v>0.70834838879211526</v>
-      </c>
-      <c r="H48" s="27">
-        <f t="shared" ca="1" si="2"/>
-        <v>619.80484019310086</v>
-      </c>
+      <c r="G48" s="27"/>
+      <c r="H48" s="27"/>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A49" s="5" t="s">
@@ -2070,14 +2016,8 @@
         <f t="shared" si="5"/>
         <v>627.08333333333337</v>
       </c>
-      <c r="G49" s="27">
-        <f t="shared" ca="1" si="1"/>
-        <v>0.68612303893942894</v>
-      </c>
-      <c r="H49" s="27">
-        <f t="shared" ca="1" si="2"/>
-        <v>600.35765907200027</v>
-      </c>
+      <c r="G49" s="27"/>
+      <c r="H49" s="27"/>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A50" s="5" t="s">
@@ -2102,14 +2042,8 @@
         <f t="shared" si="5"/>
         <v>641.66666666666663</v>
       </c>
-      <c r="G50" s="27">
-        <f t="shared" ca="1" si="1"/>
-        <v>0.73865589314218538</v>
-      </c>
-      <c r="H50" s="27">
-        <f t="shared" ca="1" si="2"/>
-        <v>646.32390649941226</v>
-      </c>
+      <c r="G50" s="27"/>
+      <c r="H50" s="27"/>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A51" s="5" t="s">
@@ -2134,14 +2068,8 @@
         <f t="shared" si="5"/>
         <v>656.25</v>
       </c>
-      <c r="G51" s="27">
-        <f t="shared" ca="1" si="1"/>
-        <v>0.73498431334333802</v>
-      </c>
-      <c r="H51" s="27">
-        <f t="shared" ca="1" si="2"/>
-        <v>643.11127417542082</v>
-      </c>
+      <c r="G51" s="27"/>
+      <c r="H51" s="27"/>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A52" s="5" t="s">
@@ -2166,14 +2094,8 @@
         <f t="shared" si="5"/>
         <v>670.83333333333337</v>
       </c>
-      <c r="G52" s="27">
-        <f t="shared" ca="1" si="1"/>
-        <v>0.80239309563934902</v>
-      </c>
-      <c r="H52" s="27">
-        <f t="shared" ca="1" si="2"/>
-        <v>702.09395868443039</v>
-      </c>
+      <c r="G52" s="27"/>
+      <c r="H52" s="27"/>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A53" s="5" t="s">
@@ -2198,14 +2120,8 @@
         <f t="shared" si="5"/>
         <v>685.41666666666663</v>
       </c>
-      <c r="G53" s="27">
-        <f t="shared" ca="1" si="1"/>
-        <v>0.77130715118020754</v>
-      </c>
-      <c r="H53" s="27">
-        <f t="shared" ca="1" si="2"/>
-        <v>674.89375728268158</v>
-      </c>
+      <c r="G53" s="27"/>
+      <c r="H53" s="27"/>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A54" s="5" t="s">
@@ -2230,14 +2146,8 @@
         <f t="shared" si="5"/>
         <v>700</v>
       </c>
-      <c r="G54" s="27">
-        <f t="shared" ca="1" si="1"/>
-        <v>0.71234225328647338</v>
-      </c>
-      <c r="H54" s="27">
-        <f t="shared" ca="1" si="2"/>
-        <v>623.29947162566418</v>
-      </c>
+      <c r="G54" s="27"/>
+      <c r="H54" s="27"/>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A55" s="5" t="s">
@@ -2262,14 +2172,8 @@
         <f t="shared" si="5"/>
         <v>714.58333333333337</v>
       </c>
-      <c r="G55" s="27">
-        <f t="shared" ca="1" si="1"/>
-        <v>0.79107228292368514</v>
-      </c>
-      <c r="H55" s="27">
-        <f t="shared" ca="1" si="2"/>
-        <v>692.18824755822448</v>
-      </c>
+      <c r="G55" s="27"/>
+      <c r="H55" s="27"/>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A56" s="5" t="s">
@@ -2294,14 +2198,8 @@
         <f t="shared" si="5"/>
         <v>729.16666666666674</v>
       </c>
-      <c r="G56" s="27">
-        <f t="shared" ca="1" si="1"/>
-        <v>0.81627690658189489</v>
-      </c>
-      <c r="H56" s="27">
-        <f t="shared" ca="1" si="2"/>
-        <v>714.24229325915803</v>
-      </c>
+      <c r="G56" s="27"/>
+      <c r="H56" s="27"/>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A57" s="5" t="s">
@@ -2326,14 +2224,8 @@
         <f t="shared" si="5"/>
         <v>743.75</v>
       </c>
-      <c r="G57" s="27">
-        <f t="shared" ca="1" si="1"/>
-        <v>0.88722716420532044</v>
-      </c>
-      <c r="H57" s="27">
-        <f t="shared" ca="1" si="2"/>
-        <v>776.32376867965536</v>
-      </c>
+      <c r="G57" s="27"/>
+      <c r="H57" s="27"/>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A58" s="5" t="s">
@@ -2358,14 +2250,8 @@
         <f t="shared" si="5"/>
         <v>758.33333333333337</v>
       </c>
-      <c r="G58" s="27">
-        <f t="shared" ca="1" si="1"/>
-        <v>0.85993266052557271</v>
-      </c>
-      <c r="H58" s="27">
-        <f t="shared" ca="1" si="2"/>
-        <v>752.44107795987611</v>
-      </c>
+      <c r="G58" s="27"/>
+      <c r="H58" s="27"/>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A59" s="5" t="s">
@@ -2390,14 +2276,8 @@
         <f t="shared" si="5"/>
         <v>772.91666666666663</v>
       </c>
-      <c r="G59" s="27">
-        <f t="shared" ca="1" si="1"/>
-        <v>0.92301435426997114</v>
-      </c>
-      <c r="H59" s="27">
-        <f t="shared" ca="1" si="2"/>
-        <v>807.6375599862248</v>
-      </c>
+      <c r="G59" s="27"/>
+      <c r="H59" s="27"/>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A60" s="5" t="s">
@@ -2422,14 +2302,8 @@
         <f t="shared" si="5"/>
         <v>787.5</v>
       </c>
-      <c r="G60" s="27">
-        <f t="shared" ca="1" si="1"/>
-        <v>0.91889349694767641</v>
-      </c>
-      <c r="H60" s="27">
-        <f t="shared" ca="1" si="2"/>
-        <v>804.03180982921685</v>
-      </c>
+      <c r="G60" s="27"/>
+      <c r="H60" s="27"/>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A61" s="5" t="s">
@@ -2454,14 +2328,8 @@
         <f t="shared" si="5"/>
         <v>802.08333333333326</v>
       </c>
-      <c r="G61" s="27">
-        <f t="shared" ca="1" si="1"/>
-        <v>0.88723153964947632</v>
-      </c>
-      <c r="H61" s="27">
-        <f t="shared" ca="1" si="2"/>
-        <v>776.32759719329181</v>
-      </c>
+      <c r="G61" s="27"/>
+      <c r="H61" s="27"/>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A62" s="5" t="s">
@@ -2486,14 +2354,8 @@
         <f t="shared" si="5"/>
         <v>816.66666666666663</v>
       </c>
-      <c r="G62" s="27">
-        <f t="shared" ca="1" si="1"/>
-        <v>0.93649298172232753</v>
-      </c>
-      <c r="H62" s="27">
-        <f t="shared" ca="1" si="2"/>
-        <v>819.43135900703658</v>
-      </c>
+      <c r="G62" s="27"/>
+      <c r="H62" s="27"/>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A63" s="5" t="s">
@@ -2518,14 +2380,8 @@
         <f t="shared" si="5"/>
         <v>831.25</v>
       </c>
-      <c r="G63" s="27">
-        <f t="shared" ca="1" si="1"/>
-        <v>0.91947715229476501</v>
-      </c>
-      <c r="H63" s="27">
-        <f t="shared" ca="1" si="2"/>
-        <v>804.54250825791939</v>
-      </c>
+      <c r="G63" s="27"/>
+      <c r="H63" s="27"/>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A64" s="5" t="s">
@@ -2550,14 +2406,8 @@
         <f t="shared" si="5"/>
         <v>845.83333333333337</v>
       </c>
-      <c r="G64" s="27">
-        <f ca="1">NORMINV(RAND(), E64, 2*1/60)</f>
-        <v>0.94264231446100177</v>
-      </c>
-      <c r="H64" s="27">
-        <f t="shared" ca="1" si="2"/>
-        <v>824.81202515337657</v>
-      </c>
+      <c r="G64" s="27"/>
+      <c r="H64" s="27"/>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A65" s="5" t="s">
@@ -2582,14 +2432,8 @@
         <f t="shared" si="5"/>
         <v>860.41666666666663</v>
       </c>
-      <c r="G65" s="27">
-        <f t="shared" ca="1" si="1"/>
-        <v>0.94539309759991152</v>
-      </c>
-      <c r="H65" s="27">
-        <f t="shared" ca="1" si="2"/>
-        <v>827.21896039992259</v>
-      </c>
+      <c r="G65" s="27"/>
+      <c r="H65" s="27"/>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A66" s="5" t="s">
@@ -2614,14 +2458,8 @@
         <f t="shared" si="5"/>
         <v>875</v>
       </c>
-      <c r="G66" s="15">
-        <f ca="1">NORMINV(RAND(), E66, 2*1/60)</f>
-        <v>0.99438873881364409</v>
-      </c>
-      <c r="H66" s="15">
-        <f t="shared" ca="1" si="2"/>
-        <v>870.09014646193862</v>
-      </c>
+      <c r="G66" s="15"/>
+      <c r="H66" s="15"/>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A67" s="5"/>

</xml_diff>

<commit_message>
Continued development of the Progress class
</commit_message>
<xml_diff>
--- a/13-ProgressReports/WP1-Prg.xlsx
+++ b/13-ProgressReports/WP1-Prg.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10708"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ken.long/KL-GIT/CCAP/02-LhARA/01-LhARA-costing-tool/13-ProgressReports/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A0C3BA7E-11D3-6E4A-B173-0FE387C8CAA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17500F3B-6D96-3444-9C83-9BA3D92B2626}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2600" yWindow="640" windowWidth="27640" windowHeight="19000" xr2:uid="{CC2CDACD-23D9-2349-BC94-9046B71DD28A}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="23">
   <si>
     <t>Date:</t>
   </si>
@@ -590,10 +590,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B830DFFD-7C49-A743-A7AB-F5C942B0BCC3}">
-  <dimension ref="A1:H34"/>
+  <dimension ref="A1:H70"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -719,15 +719,21 @@
         <v>44866</v>
       </c>
       <c r="E7" s="27">
-        <f>C7/24</f>
-        <v>4.1666666666666664E-2</v>
+        <f>C7/60</f>
+        <v>1.6666666666666666E-2</v>
       </c>
       <c r="F7" s="27">
-        <f>E7*192</f>
-        <v>8</v>
-      </c>
-      <c r="G7" s="27"/>
-      <c r="H7" s="27"/>
+        <f>E7*875</f>
+        <v>14.583333333333334</v>
+      </c>
+      <c r="G7" s="27">
+        <f ca="1">ABS(NORMINV(RAND(), E7, 2*1/60))</f>
+        <v>2.5733075649297804E-2</v>
+      </c>
+      <c r="H7" s="27">
+        <f ca="1">G7*875</f>
+        <v>22.516441193135577</v>
+      </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
@@ -745,15 +751,21 @@
         <v>44927</v>
       </c>
       <c r="E8" s="27">
-        <f t="shared" ref="E8:E29" si="0">C8/24</f>
-        <v>8.3333333333333329E-2</v>
+        <f t="shared" ref="E8:E65" si="0">C8/60</f>
+        <v>3.3333333333333333E-2</v>
       </c>
       <c r="F8" s="27">
-        <f t="shared" ref="F8:F29" si="1">E8*192</f>
-        <v>16</v>
-      </c>
-      <c r="G8" s="27"/>
-      <c r="H8" s="27"/>
+        <f>E8*875</f>
+        <v>29.166666666666668</v>
+      </c>
+      <c r="G8" s="27">
+        <f t="shared" ref="G8:G65" ca="1" si="1">NORMINV(RAND(), E8, 2*1/60)</f>
+        <v>4.8229416718184238E-2</v>
+      </c>
+      <c r="H8" s="27">
+        <f t="shared" ref="H8:H66" ca="1" si="2">G8*875</f>
+        <v>42.200739628411206</v>
+      </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
@@ -763,23 +775,29 @@
         <v>12</v>
       </c>
       <c r="C9" s="24">
-        <f t="shared" ref="C9:C29" si="2">C8+1</f>
+        <f t="shared" ref="C9:C65" si="3">C8+1</f>
         <v>3</v>
       </c>
       <c r="D9" s="20">
-        <f t="shared" ref="D9:D16" si="3">EDATE($D$7,C9)</f>
+        <f t="shared" ref="D9:D65" si="4">EDATE($D$7,C9)</f>
         <v>44958</v>
       </c>
       <c r="E9" s="27">
         <f t="shared" si="0"/>
-        <v>0.125</v>
+        <v>0.05</v>
       </c>
       <c r="F9" s="27">
-        <f t="shared" si="1"/>
-        <v>24</v>
-      </c>
-      <c r="G9" s="27"/>
-      <c r="H9" s="27"/>
+        <f t="shared" ref="F8:F66" si="5">E9*875</f>
+        <v>43.75</v>
+      </c>
+      <c r="G9" s="27">
+        <f t="shared" ca="1" si="1"/>
+        <v>1.2302757772623761E-2</v>
+      </c>
+      <c r="H9" s="27">
+        <f t="shared" ca="1" si="2"/>
+        <v>10.764913051045792</v>
+      </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="s">
@@ -789,23 +807,29 @@
         <v>12</v>
       </c>
       <c r="C10" s="24">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>4</v>
       </c>
       <c r="D10" s="20">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>44986</v>
       </c>
       <c r="E10" s="27">
         <f t="shared" si="0"/>
-        <v>0.16666666666666666</v>
+        <v>6.6666666666666666E-2</v>
       </c>
       <c r="F10" s="27">
-        <f t="shared" si="1"/>
-        <v>32</v>
-      </c>
-      <c r="G10" s="27"/>
-      <c r="H10" s="27"/>
+        <f t="shared" si="5"/>
+        <v>58.333333333333336</v>
+      </c>
+      <c r="G10" s="27">
+        <f t="shared" ca="1" si="1"/>
+        <v>7.9236599742196656E-2</v>
+      </c>
+      <c r="H10" s="27">
+        <f t="shared" ca="1" si="2"/>
+        <v>69.332024774422081</v>
+      </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" s="5" t="s">
@@ -815,23 +839,29 @@
         <v>12</v>
       </c>
       <c r="C11" s="24">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>5</v>
       </c>
       <c r="D11" s="20">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>45017</v>
       </c>
       <c r="E11" s="27">
         <f t="shared" si="0"/>
-        <v>0.20833333333333334</v>
+        <v>8.3333333333333329E-2</v>
       </c>
       <c r="F11" s="27">
-        <f t="shared" si="1"/>
-        <v>40</v>
-      </c>
-      <c r="G11" s="27"/>
-      <c r="H11" s="27"/>
+        <f t="shared" si="5"/>
+        <v>72.916666666666657</v>
+      </c>
+      <c r="G11" s="27">
+        <f t="shared" ca="1" si="1"/>
+        <v>5.0500202758635586E-2</v>
+      </c>
+      <c r="H11" s="27">
+        <f t="shared" ca="1" si="2"/>
+        <v>44.187677413806135</v>
+      </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" s="5" t="s">
@@ -841,23 +871,29 @@
         <v>12</v>
       </c>
       <c r="C12" s="24">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>6</v>
       </c>
       <c r="D12" s="20">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>45047</v>
       </c>
       <c r="E12" s="27">
         <f t="shared" si="0"/>
-        <v>0.25</v>
+        <v>0.1</v>
       </c>
       <c r="F12" s="27">
-        <f t="shared" si="1"/>
-        <v>48</v>
-      </c>
-      <c r="G12" s="27"/>
-      <c r="H12" s="27"/>
+        <f t="shared" si="5"/>
+        <v>87.5</v>
+      </c>
+      <c r="G12" s="27">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.12316662137289992</v>
+      </c>
+      <c r="H12" s="27">
+        <f t="shared" ca="1" si="2"/>
+        <v>107.77079370128743</v>
+      </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" s="5" t="s">
@@ -867,23 +903,29 @@
         <v>12</v>
       </c>
       <c r="C13" s="24">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>7</v>
       </c>
       <c r="D13" s="20">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>45078</v>
       </c>
       <c r="E13" s="27">
         <f t="shared" si="0"/>
-        <v>0.29166666666666669</v>
+        <v>0.11666666666666667</v>
       </c>
       <c r="F13" s="27">
-        <f t="shared" si="1"/>
-        <v>56</v>
-      </c>
-      <c r="G13" s="27"/>
-      <c r="H13" s="27"/>
+        <f t="shared" si="5"/>
+        <v>102.08333333333333</v>
+      </c>
+      <c r="G13" s="27">
+        <f t="shared" ca="1" si="1"/>
+        <v>9.822022495821775E-2</v>
+      </c>
+      <c r="H13" s="27">
+        <f t="shared" ca="1" si="2"/>
+        <v>85.942696838440526</v>
+      </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" s="5" t="s">
@@ -893,23 +935,29 @@
         <v>12</v>
       </c>
       <c r="C14" s="24">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>8</v>
       </c>
       <c r="D14" s="20">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>45108</v>
       </c>
       <c r="E14" s="27">
         <f t="shared" si="0"/>
-        <v>0.33333333333333331</v>
+        <v>0.13333333333333333</v>
       </c>
       <c r="F14" s="27">
-        <f t="shared" si="1"/>
-        <v>64</v>
-      </c>
-      <c r="G14" s="27"/>
-      <c r="H14" s="27"/>
+        <f t="shared" si="5"/>
+        <v>116.66666666666667</v>
+      </c>
+      <c r="G14" s="27">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.15447590322025012</v>
+      </c>
+      <c r="H14" s="27">
+        <f t="shared" ca="1" si="2"/>
+        <v>135.16641531771884</v>
+      </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" s="5" t="s">
@@ -919,23 +967,29 @@
         <v>12</v>
       </c>
       <c r="C15" s="24">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>9</v>
       </c>
       <c r="D15" s="20">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>45139</v>
       </c>
       <c r="E15" s="27">
         <f t="shared" si="0"/>
-        <v>0.375</v>
+        <v>0.15</v>
       </c>
       <c r="F15" s="27">
-        <f t="shared" si="1"/>
-        <v>72</v>
-      </c>
-      <c r="G15" s="27"/>
-      <c r="H15" s="27"/>
+        <f t="shared" si="5"/>
+        <v>131.25</v>
+      </c>
+      <c r="G15" s="27">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.15704994880771705</v>
+      </c>
+      <c r="H15" s="27">
+        <f t="shared" ca="1" si="2"/>
+        <v>137.41870520675243</v>
+      </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" s="5" t="s">
@@ -945,23 +999,29 @@
         <v>12</v>
       </c>
       <c r="C16" s="24">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>10</v>
       </c>
       <c r="D16" s="20">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>45170</v>
       </c>
       <c r="E16" s="27">
         <f t="shared" si="0"/>
-        <v>0.41666666666666669</v>
+        <v>0.16666666666666666</v>
       </c>
       <c r="F16" s="27">
-        <f t="shared" si="1"/>
-        <v>80</v>
-      </c>
-      <c r="G16" s="27"/>
-      <c r="H16" s="27"/>
+        <f t="shared" si="5"/>
+        <v>145.83333333333331</v>
+      </c>
+      <c r="G16" s="27">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.18705068720235496</v>
+      </c>
+      <c r="H16" s="27">
+        <f t="shared" ca="1" si="2"/>
+        <v>163.66935130206059</v>
+      </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" s="5" t="s">
@@ -971,23 +1031,29 @@
         <v>12</v>
       </c>
       <c r="C17" s="24">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>11</v>
       </c>
       <c r="D17" s="20">
-        <f t="shared" ref="D17:D29" si="4">EDATE($D$7,C17)</f>
+        <f t="shared" ref="D17:D49" si="6">EDATE($D$7,C17)</f>
         <v>45200</v>
       </c>
       <c r="E17" s="27">
-        <f t="shared" si="0"/>
-        <v>0.45833333333333331</v>
+        <f t="shared" ref="E17:E49" si="7">C17/60</f>
+        <v>0.18333333333333332</v>
       </c>
       <c r="F17" s="27">
-        <f t="shared" si="1"/>
-        <v>88</v>
-      </c>
-      <c r="G17" s="27"/>
-      <c r="H17" s="27"/>
+        <f t="shared" si="5"/>
+        <v>160.41666666666666</v>
+      </c>
+      <c r="G17" s="27">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.21130250852998642</v>
+      </c>
+      <c r="H17" s="27">
+        <f t="shared" ca="1" si="2"/>
+        <v>184.88969496373812</v>
+      </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" s="5" t="s">
@@ -997,23 +1063,29 @@
         <v>12</v>
       </c>
       <c r="C18" s="24">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>12</v>
       </c>
       <c r="D18" s="20">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>45231</v>
       </c>
       <c r="E18" s="27">
-        <f t="shared" si="0"/>
-        <v>0.5</v>
+        <f t="shared" si="7"/>
+        <v>0.2</v>
       </c>
       <c r="F18" s="27">
-        <f t="shared" si="1"/>
-        <v>96</v>
-      </c>
-      <c r="G18" s="27"/>
-      <c r="H18" s="27"/>
+        <f t="shared" si="5"/>
+        <v>175</v>
+      </c>
+      <c r="G18" s="27">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.18440657297535784</v>
+      </c>
+      <c r="H18" s="27">
+        <f t="shared" ca="1" si="2"/>
+        <v>161.35575135343811</v>
+      </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" s="5" t="s">
@@ -1023,23 +1095,29 @@
         <v>12</v>
       </c>
       <c r="C19" s="24">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>13</v>
       </c>
       <c r="D19" s="20">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>45261</v>
       </c>
       <c r="E19" s="27">
-        <f t="shared" si="0"/>
-        <v>0.54166666666666663</v>
+        <f t="shared" si="7"/>
+        <v>0.21666666666666667</v>
       </c>
       <c r="F19" s="27">
-        <f t="shared" si="1"/>
-        <v>104</v>
-      </c>
-      <c r="G19" s="27"/>
-      <c r="H19" s="27"/>
+        <f t="shared" si="5"/>
+        <v>189.58333333333334</v>
+      </c>
+      <c r="G19" s="27">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.23110612182937737</v>
+      </c>
+      <c r="H19" s="27">
+        <f t="shared" ca="1" si="2"/>
+        <v>202.2178566007052</v>
+      </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" s="5" t="s">
@@ -1049,23 +1127,29 @@
         <v>12</v>
       </c>
       <c r="C20" s="24">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>14</v>
       </c>
       <c r="D20" s="20">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>45292</v>
       </c>
       <c r="E20" s="27">
-        <f t="shared" si="0"/>
-        <v>0.58333333333333337</v>
+        <f t="shared" si="7"/>
+        <v>0.23333333333333334</v>
       </c>
       <c r="F20" s="27">
-        <f t="shared" si="1"/>
-        <v>112</v>
-      </c>
-      <c r="G20" s="27"/>
-      <c r="H20" s="27"/>
+        <f t="shared" si="5"/>
+        <v>204.16666666666666</v>
+      </c>
+      <c r="G20" s="27">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.24759780924842345</v>
+      </c>
+      <c r="H20" s="27">
+        <f t="shared" ca="1" si="2"/>
+        <v>216.64808309237051</v>
+      </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" s="5" t="s">
@@ -1075,23 +1159,29 @@
         <v>12</v>
       </c>
       <c r="C21" s="24">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>15</v>
       </c>
       <c r="D21" s="20">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>45323</v>
       </c>
       <c r="E21" s="27">
-        <f t="shared" si="0"/>
-        <v>0.625</v>
+        <f t="shared" si="7"/>
+        <v>0.25</v>
       </c>
       <c r="F21" s="27">
-        <f t="shared" si="1"/>
-        <v>120</v>
-      </c>
-      <c r="G21" s="27"/>
-      <c r="H21" s="27"/>
+        <f t="shared" si="5"/>
+        <v>218.75</v>
+      </c>
+      <c r="G21" s="27">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.29165694972861805</v>
+      </c>
+      <c r="H21" s="27">
+        <f t="shared" ca="1" si="2"/>
+        <v>255.19983101254078</v>
+      </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" s="5" t="s">
@@ -1101,23 +1191,29 @@
         <v>12</v>
       </c>
       <c r="C22" s="24">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>16</v>
       </c>
       <c r="D22" s="20">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>45352</v>
       </c>
       <c r="E22" s="27">
-        <f t="shared" si="0"/>
-        <v>0.66666666666666663</v>
+        <f t="shared" si="7"/>
+        <v>0.26666666666666666</v>
       </c>
       <c r="F22" s="27">
-        <f t="shared" si="1"/>
-        <v>128</v>
-      </c>
-      <c r="G22" s="27"/>
-      <c r="H22" s="27"/>
+        <f t="shared" si="5"/>
+        <v>233.33333333333334</v>
+      </c>
+      <c r="G22" s="27">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.26188477434688234</v>
+      </c>
+      <c r="H22" s="27">
+        <f t="shared" ca="1" si="2"/>
+        <v>229.14917755352204</v>
+      </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" s="5" t="s">
@@ -1127,23 +1223,29 @@
         <v>12</v>
       </c>
       <c r="C23" s="24">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>17</v>
       </c>
       <c r="D23" s="20">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>45383</v>
       </c>
       <c r="E23" s="27">
-        <f t="shared" si="0"/>
-        <v>0.70833333333333337</v>
+        <f t="shared" si="7"/>
+        <v>0.28333333333333333</v>
       </c>
       <c r="F23" s="27">
-        <f t="shared" si="1"/>
-        <v>136</v>
-      </c>
-      <c r="G23" s="27"/>
-      <c r="H23" s="27"/>
+        <f t="shared" si="5"/>
+        <v>247.91666666666666</v>
+      </c>
+      <c r="G23" s="27">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.30523178213583946</v>
+      </c>
+      <c r="H23" s="27">
+        <f t="shared" ca="1" si="2"/>
+        <v>267.0778093688595</v>
+      </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" s="5" t="s">
@@ -1153,193 +1255,1387 @@
         <v>12</v>
       </c>
       <c r="C24" s="24">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>18</v>
       </c>
       <c r="D24" s="20">
+        <f t="shared" si="6"/>
+        <v>45413</v>
+      </c>
+      <c r="E24" s="27">
+        <f t="shared" si="7"/>
+        <v>0.3</v>
+      </c>
+      <c r="F24" s="27">
+        <f t="shared" si="5"/>
+        <v>262.5</v>
+      </c>
+      <c r="G24" s="27">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.33654157123855077</v>
+      </c>
+      <c r="H24" s="27">
+        <f t="shared" ca="1" si="2"/>
+        <v>294.47387483373194</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A25" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B25" s="26" t="s">
+        <v>12</v>
+      </c>
+      <c r="C25" s="24">
+        <f t="shared" si="3"/>
+        <v>19</v>
+      </c>
+      <c r="D25" s="20">
+        <f t="shared" si="6"/>
+        <v>45444</v>
+      </c>
+      <c r="E25" s="27">
+        <f t="shared" si="7"/>
+        <v>0.31666666666666665</v>
+      </c>
+      <c r="F25" s="27">
+        <f t="shared" si="5"/>
+        <v>277.08333333333331</v>
+      </c>
+      <c r="G25" s="27">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.41879273677736828</v>
+      </c>
+      <c r="H25" s="27">
+        <f t="shared" ca="1" si="2"/>
+        <v>366.44364468019722</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A26" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B26" s="26" t="s">
+        <v>12</v>
+      </c>
+      <c r="C26" s="24">
+        <f t="shared" si="3"/>
+        <v>20</v>
+      </c>
+      <c r="D26" s="20">
+        <f t="shared" si="6"/>
+        <v>45474</v>
+      </c>
+      <c r="E26" s="27">
+        <f t="shared" si="7"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="F26" s="27">
+        <f t="shared" si="5"/>
+        <v>291.66666666666663</v>
+      </c>
+      <c r="G26" s="27">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.34178412000500313</v>
+      </c>
+      <c r="H26" s="27">
+        <f t="shared" ca="1" si="2"/>
+        <v>299.06110500437774</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A27" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B27" s="26" t="s">
+        <v>12</v>
+      </c>
+      <c r="C27" s="24">
+        <f t="shared" si="3"/>
+        <v>21</v>
+      </c>
+      <c r="D27" s="20">
+        <f t="shared" si="6"/>
+        <v>45505</v>
+      </c>
+      <c r="E27" s="27">
+        <f t="shared" si="7"/>
+        <v>0.35</v>
+      </c>
+      <c r="F27" s="27">
+        <f t="shared" si="5"/>
+        <v>306.25</v>
+      </c>
+      <c r="G27" s="27">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.41028889721052142</v>
+      </c>
+      <c r="H27" s="27">
+        <f t="shared" ca="1" si="2"/>
+        <v>359.00278505920625</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A28" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B28" s="26" t="s">
+        <v>12</v>
+      </c>
+      <c r="C28" s="24">
+        <f t="shared" si="3"/>
+        <v>22</v>
+      </c>
+      <c r="D28" s="20">
+        <f t="shared" si="6"/>
+        <v>45536</v>
+      </c>
+      <c r="E28" s="27">
+        <f t="shared" si="7"/>
+        <v>0.36666666666666664</v>
+      </c>
+      <c r="F28" s="27">
+        <f t="shared" si="5"/>
+        <v>320.83333333333331</v>
+      </c>
+      <c r="G28" s="27">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.35249927827302224</v>
+      </c>
+      <c r="H28" s="27">
+        <f t="shared" ca="1" si="2"/>
+        <v>308.43686848889445</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A29" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B29" s="26" t="s">
+        <v>12</v>
+      </c>
+      <c r="C29" s="24">
+        <f t="shared" si="3"/>
+        <v>23</v>
+      </c>
+      <c r="D29" s="20">
+        <f t="shared" si="6"/>
+        <v>45566</v>
+      </c>
+      <c r="E29" s="27">
+        <f t="shared" si="7"/>
+        <v>0.38333333333333336</v>
+      </c>
+      <c r="F29" s="27">
+        <f t="shared" si="5"/>
+        <v>335.41666666666669</v>
+      </c>
+      <c r="G29" s="27">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.39056996865774546</v>
+      </c>
+      <c r="H29" s="27">
+        <f t="shared" ca="1" si="2"/>
+        <v>341.74872257552727</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A30" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B30" s="26" t="s">
+        <v>12</v>
+      </c>
+      <c r="C30" s="24">
+        <f t="shared" si="3"/>
+        <v>24</v>
+      </c>
+      <c r="D30" s="20">
+        <f t="shared" si="6"/>
+        <v>45597</v>
+      </c>
+      <c r="E30" s="27">
+        <f t="shared" si="7"/>
+        <v>0.4</v>
+      </c>
+      <c r="F30" s="27">
+        <f t="shared" si="5"/>
+        <v>350</v>
+      </c>
+      <c r="G30" s="27">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.38101714602324604</v>
+      </c>
+      <c r="H30" s="27">
+        <f t="shared" ca="1" si="2"/>
+        <v>333.39000277034029</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A31" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B31" s="26" t="s">
+        <v>12</v>
+      </c>
+      <c r="C31" s="24">
+        <f t="shared" si="3"/>
+        <v>25</v>
+      </c>
+      <c r="D31" s="20">
+        <f t="shared" si="6"/>
+        <v>45627</v>
+      </c>
+      <c r="E31" s="27">
+        <f t="shared" si="7"/>
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="F31" s="27">
+        <f t="shared" si="5"/>
+        <v>364.58333333333337</v>
+      </c>
+      <c r="G31" s="27">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.39178456467072509</v>
+      </c>
+      <c r="H31" s="27">
+        <f t="shared" ca="1" si="2"/>
+        <v>342.81149408688447</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A32" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B32" s="26" t="s">
+        <v>12</v>
+      </c>
+      <c r="C32" s="24">
+        <f t="shared" si="3"/>
+        <v>26</v>
+      </c>
+      <c r="D32" s="20">
+        <f t="shared" si="6"/>
+        <v>45658</v>
+      </c>
+      <c r="E32" s="27">
+        <f t="shared" si="7"/>
+        <v>0.43333333333333335</v>
+      </c>
+      <c r="F32" s="27">
+        <f t="shared" si="5"/>
+        <v>379.16666666666669</v>
+      </c>
+      <c r="G32" s="27">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.44308129592774714</v>
+      </c>
+      <c r="H32" s="27">
+        <f t="shared" ca="1" si="2"/>
+        <v>387.69613393677872</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A33" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B33" s="26" t="s">
+        <v>12</v>
+      </c>
+      <c r="C33" s="24">
+        <f t="shared" si="3"/>
+        <v>27</v>
+      </c>
+      <c r="D33" s="20">
+        <f t="shared" si="6"/>
+        <v>45689</v>
+      </c>
+      <c r="E33" s="27">
+        <f t="shared" si="7"/>
+        <v>0.45</v>
+      </c>
+      <c r="F33" s="27">
+        <f t="shared" si="5"/>
+        <v>393.75</v>
+      </c>
+      <c r="G33" s="27">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.44293035923880925</v>
+      </c>
+      <c r="H33" s="27">
+        <f t="shared" ca="1" si="2"/>
+        <v>387.56406433395807</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A34" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B34" s="26" t="s">
+        <v>12</v>
+      </c>
+      <c r="C34" s="24">
+        <f t="shared" si="3"/>
+        <v>28</v>
+      </c>
+      <c r="D34" s="20">
+        <f t="shared" si="6"/>
+        <v>45717</v>
+      </c>
+      <c r="E34" s="27">
+        <f t="shared" si="7"/>
+        <v>0.46666666666666667</v>
+      </c>
+      <c r="F34" s="27">
+        <f t="shared" si="5"/>
+        <v>408.33333333333331</v>
+      </c>
+      <c r="G34" s="27">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.42055197158333757</v>
+      </c>
+      <c r="H34" s="27">
+        <f t="shared" ca="1" si="2"/>
+        <v>367.98297513542036</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A35" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B35" s="26" t="s">
+        <v>12</v>
+      </c>
+      <c r="C35" s="24">
+        <f t="shared" si="3"/>
+        <v>29</v>
+      </c>
+      <c r="D35" s="20">
+        <f t="shared" si="6"/>
+        <v>45748</v>
+      </c>
+      <c r="E35" s="27">
+        <f t="shared" si="7"/>
+        <v>0.48333333333333334</v>
+      </c>
+      <c r="F35" s="27">
+        <f t="shared" si="5"/>
+        <v>422.91666666666669</v>
+      </c>
+      <c r="G35" s="27">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.42888661826032265</v>
+      </c>
+      <c r="H35" s="27">
+        <f t="shared" ca="1" si="2"/>
+        <v>375.27579097778232</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A36" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B36" s="26" t="s">
+        <v>12</v>
+      </c>
+      <c r="C36" s="24">
+        <f t="shared" si="3"/>
+        <v>30</v>
+      </c>
+      <c r="D36" s="20">
+        <f t="shared" si="6"/>
+        <v>45778</v>
+      </c>
+      <c r="E36" s="27">
+        <f t="shared" si="7"/>
+        <v>0.5</v>
+      </c>
+      <c r="F36" s="27">
+        <f t="shared" si="5"/>
+        <v>437.5</v>
+      </c>
+      <c r="G36" s="27">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.53989448370900195</v>
+      </c>
+      <c r="H36" s="27">
+        <f t="shared" ca="1" si="2"/>
+        <v>472.40767324537671</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A37" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B37" s="26" t="s">
+        <v>12</v>
+      </c>
+      <c r="C37" s="24">
+        <f t="shared" si="3"/>
+        <v>31</v>
+      </c>
+      <c r="D37" s="20">
+        <f t="shared" si="6"/>
+        <v>45809</v>
+      </c>
+      <c r="E37" s="27">
+        <f t="shared" si="7"/>
+        <v>0.51666666666666672</v>
+      </c>
+      <c r="F37" s="27">
+        <f t="shared" si="5"/>
+        <v>452.08333333333337</v>
+      </c>
+      <c r="G37" s="27">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.51701251730873432</v>
+      </c>
+      <c r="H37" s="27">
+        <f t="shared" ca="1" si="2"/>
+        <v>452.38595264514254</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A38" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B38" s="26" t="s">
+        <v>12</v>
+      </c>
+      <c r="C38" s="24">
+        <f t="shared" si="3"/>
+        <v>32</v>
+      </c>
+      <c r="D38" s="20">
+        <f t="shared" si="6"/>
+        <v>45839</v>
+      </c>
+      <c r="E38" s="27">
+        <f t="shared" si="7"/>
+        <v>0.53333333333333333</v>
+      </c>
+      <c r="F38" s="27">
+        <f t="shared" si="5"/>
+        <v>466.66666666666669</v>
+      </c>
+      <c r="G38" s="27">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.52110224311108622</v>
+      </c>
+      <c r="H38" s="27">
+        <f t="shared" ca="1" si="2"/>
+        <v>455.96446272220044</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A39" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B39" s="26" t="s">
+        <v>12</v>
+      </c>
+      <c r="C39" s="24">
+        <f t="shared" si="3"/>
+        <v>33</v>
+      </c>
+      <c r="D39" s="20">
+        <f t="shared" si="6"/>
+        <v>45870</v>
+      </c>
+      <c r="E39" s="27">
+        <f t="shared" si="7"/>
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="F39" s="27">
+        <f t="shared" si="5"/>
+        <v>481.25000000000006</v>
+      </c>
+      <c r="G39" s="27">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.58234871085756135</v>
+      </c>
+      <c r="H39" s="27">
+        <f t="shared" ca="1" si="2"/>
+        <v>509.55512200036617</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A40" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B40" s="26" t="s">
+        <v>12</v>
+      </c>
+      <c r="C40" s="24">
+        <f t="shared" si="3"/>
+        <v>34</v>
+      </c>
+      <c r="D40" s="20">
+        <f t="shared" si="6"/>
+        <v>45901</v>
+      </c>
+      <c r="E40" s="27">
+        <f t="shared" si="7"/>
+        <v>0.56666666666666665</v>
+      </c>
+      <c r="F40" s="27">
+        <f t="shared" si="5"/>
+        <v>495.83333333333331</v>
+      </c>
+      <c r="G40" s="27">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.61637293306726582</v>
+      </c>
+      <c r="H40" s="27">
+        <f t="shared" ca="1" si="2"/>
+        <v>539.32631643385764</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A41" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B41" s="26" t="s">
+        <v>12</v>
+      </c>
+      <c r="C41" s="24">
+        <f t="shared" si="3"/>
+        <v>35</v>
+      </c>
+      <c r="D41" s="20">
+        <f t="shared" si="6"/>
+        <v>45931</v>
+      </c>
+      <c r="E41" s="27">
+        <f t="shared" si="7"/>
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="F41" s="27">
+        <f t="shared" si="5"/>
+        <v>510.41666666666669</v>
+      </c>
+      <c r="G41" s="27">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.65756062482076616</v>
+      </c>
+      <c r="H41" s="27">
+        <f t="shared" ca="1" si="2"/>
+        <v>575.36554671817044</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A42" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B42" s="26" t="s">
+        <v>12</v>
+      </c>
+      <c r="C42" s="24">
+        <f t="shared" si="3"/>
+        <v>36</v>
+      </c>
+      <c r="D42" s="20">
+        <f t="shared" si="6"/>
+        <v>45962</v>
+      </c>
+      <c r="E42" s="27">
+        <f t="shared" si="7"/>
+        <v>0.6</v>
+      </c>
+      <c r="F42" s="27">
+        <f t="shared" si="5"/>
+        <v>525</v>
+      </c>
+      <c r="G42" s="27">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.52754172486701056</v>
+      </c>
+      <c r="H42" s="27">
+        <f t="shared" ca="1" si="2"/>
+        <v>461.59900925863423</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A43" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B43" s="26" t="s">
+        <v>12</v>
+      </c>
+      <c r="C43" s="24">
+        <f t="shared" si="3"/>
+        <v>37</v>
+      </c>
+      <c r="D43" s="20">
+        <f t="shared" si="6"/>
+        <v>45992</v>
+      </c>
+      <c r="E43" s="27">
+        <f t="shared" si="7"/>
+        <v>0.6166666666666667</v>
+      </c>
+      <c r="F43" s="27">
+        <f t="shared" si="5"/>
+        <v>539.58333333333337</v>
+      </c>
+      <c r="G43" s="27">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.62080674881166131</v>
+      </c>
+      <c r="H43" s="27">
+        <f t="shared" ca="1" si="2"/>
+        <v>543.2059052102037</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A44" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B44" s="26" t="s">
+        <v>12</v>
+      </c>
+      <c r="C44" s="24">
+        <f t="shared" si="3"/>
+        <v>38</v>
+      </c>
+      <c r="D44" s="20">
+        <f t="shared" si="6"/>
+        <v>46023</v>
+      </c>
+      <c r="E44" s="27">
+        <f t="shared" si="7"/>
+        <v>0.6333333333333333</v>
+      </c>
+      <c r="F44" s="27">
+        <f t="shared" si="5"/>
+        <v>554.16666666666663</v>
+      </c>
+      <c r="G44" s="27">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.59520759372053766</v>
+      </c>
+      <c r="H44" s="27">
+        <f t="shared" ca="1" si="2"/>
+        <v>520.80664450547044</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A45" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B45" s="26" t="s">
+        <v>12</v>
+      </c>
+      <c r="C45" s="24">
+        <f t="shared" si="3"/>
+        <v>39</v>
+      </c>
+      <c r="D45" s="20">
+        <f t="shared" si="6"/>
+        <v>46054</v>
+      </c>
+      <c r="E45" s="27">
+        <f t="shared" si="7"/>
+        <v>0.65</v>
+      </c>
+      <c r="F45" s="27">
+        <f t="shared" si="5"/>
+        <v>568.75</v>
+      </c>
+      <c r="G45" s="27">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.69575655859136842</v>
+      </c>
+      <c r="H45" s="27">
+        <f t="shared" ca="1" si="2"/>
+        <v>608.78698876744738</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A46" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B46" s="26" t="s">
+        <v>12</v>
+      </c>
+      <c r="C46" s="24">
+        <f t="shared" si="3"/>
+        <v>40</v>
+      </c>
+      <c r="D46" s="20">
+        <f t="shared" si="6"/>
+        <v>46082</v>
+      </c>
+      <c r="E46" s="27">
+        <f t="shared" si="7"/>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="F46" s="27">
+        <f t="shared" si="5"/>
+        <v>583.33333333333326</v>
+      </c>
+      <c r="G46" s="27">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.68021193152482806</v>
+      </c>
+      <c r="H46" s="27">
+        <f t="shared" ca="1" si="2"/>
+        <v>595.18544008422452</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A47" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B47" s="26" t="s">
+        <v>12</v>
+      </c>
+      <c r="C47" s="24">
+        <f t="shared" si="3"/>
+        <v>41</v>
+      </c>
+      <c r="D47" s="20">
+        <f t="shared" si="6"/>
+        <v>46113</v>
+      </c>
+      <c r="E47" s="27">
+        <f t="shared" si="7"/>
+        <v>0.68333333333333335</v>
+      </c>
+      <c r="F47" s="27">
+        <f t="shared" si="5"/>
+        <v>597.91666666666663</v>
+      </c>
+      <c r="G47" s="27">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.72523840220572677</v>
+      </c>
+      <c r="H47" s="27">
+        <f t="shared" ca="1" si="2"/>
+        <v>634.5836019300109</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A48" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B48" s="26" t="s">
+        <v>12</v>
+      </c>
+      <c r="C48" s="24">
+        <f t="shared" si="3"/>
+        <v>42</v>
+      </c>
+      <c r="D48" s="20">
+        <f t="shared" si="6"/>
+        <v>46143</v>
+      </c>
+      <c r="E48" s="27">
+        <f t="shared" si="7"/>
+        <v>0.7</v>
+      </c>
+      <c r="F48" s="27">
+        <f t="shared" si="5"/>
+        <v>612.5</v>
+      </c>
+      <c r="G48" s="27">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.70834838879211526</v>
+      </c>
+      <c r="H48" s="27">
+        <f t="shared" ca="1" si="2"/>
+        <v>619.80484019310086</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A49" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B49" s="26" t="s">
+        <v>12</v>
+      </c>
+      <c r="C49" s="24">
+        <f t="shared" si="3"/>
+        <v>43</v>
+      </c>
+      <c r="D49" s="20">
+        <f t="shared" si="6"/>
+        <v>46174</v>
+      </c>
+      <c r="E49" s="27">
+        <f t="shared" si="7"/>
+        <v>0.71666666666666667</v>
+      </c>
+      <c r="F49" s="27">
+        <f t="shared" si="5"/>
+        <v>627.08333333333337</v>
+      </c>
+      <c r="G49" s="27">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.68612303893942894</v>
+      </c>
+      <c r="H49" s="27">
+        <f t="shared" ca="1" si="2"/>
+        <v>600.35765907200027</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A50" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B50" s="26" t="s">
+        <v>12</v>
+      </c>
+      <c r="C50" s="24">
+        <f t="shared" si="3"/>
+        <v>44</v>
+      </c>
+      <c r="D50" s="20">
         <f t="shared" si="4"/>
-        <v>45413</v>
-      </c>
-      <c r="E24" s="27">
+        <v>46204</v>
+      </c>
+      <c r="E50" s="27">
+        <f t="shared" si="0"/>
+        <v>0.73333333333333328</v>
+      </c>
+      <c r="F50" s="27">
+        <f t="shared" si="5"/>
+        <v>641.66666666666663</v>
+      </c>
+      <c r="G50" s="27">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.73865589314218538</v>
+      </c>
+      <c r="H50" s="27">
+        <f t="shared" ca="1" si="2"/>
+        <v>646.32390649941226</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A51" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B51" s="26" t="s">
+        <v>12</v>
+      </c>
+      <c r="C51" s="24">
+        <f t="shared" si="3"/>
+        <v>45</v>
+      </c>
+      <c r="D51" s="20">
+        <f t="shared" si="4"/>
+        <v>46235</v>
+      </c>
+      <c r="E51" s="27">
         <f t="shared" si="0"/>
         <v>0.75</v>
       </c>
-      <c r="F24" s="27">
-        <f t="shared" si="1"/>
-        <v>144</v>
-      </c>
-      <c r="G24" s="27"/>
-      <c r="H24" s="27"/>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A25" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="B25" s="26" t="s">
-        <v>12</v>
-      </c>
-      <c r="C25" s="24">
-        <f t="shared" si="2"/>
-        <v>19</v>
-      </c>
-      <c r="D25" s="20">
+      <c r="F51" s="27">
+        <f t="shared" si="5"/>
+        <v>656.25</v>
+      </c>
+      <c r="G51" s="27">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.73498431334333802</v>
+      </c>
+      <c r="H51" s="27">
+        <f t="shared" ca="1" si="2"/>
+        <v>643.11127417542082</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A52" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B52" s="26" t="s">
+        <v>12</v>
+      </c>
+      <c r="C52" s="24">
+        <f t="shared" si="3"/>
+        <v>46</v>
+      </c>
+      <c r="D52" s="20">
         <f t="shared" si="4"/>
-        <v>45444</v>
-      </c>
-      <c r="E25" s="27">
+        <v>46266</v>
+      </c>
+      <c r="E52" s="27">
         <f t="shared" si="0"/>
-        <v>0.79166666666666663</v>
-      </c>
-      <c r="F25" s="27">
-        <f t="shared" si="1"/>
-        <v>152</v>
-      </c>
-      <c r="G25" s="27"/>
-      <c r="H25" s="27"/>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A26" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="B26" s="26" t="s">
-        <v>12</v>
-      </c>
-      <c r="C26" s="24">
-        <f t="shared" si="2"/>
-        <v>20</v>
-      </c>
-      <c r="D26" s="20">
+        <v>0.76666666666666672</v>
+      </c>
+      <c r="F52" s="27">
+        <f t="shared" si="5"/>
+        <v>670.83333333333337</v>
+      </c>
+      <c r="G52" s="27">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.80239309563934902</v>
+      </c>
+      <c r="H52" s="27">
+        <f t="shared" ca="1" si="2"/>
+        <v>702.09395868443039</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A53" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B53" s="26" t="s">
+        <v>12</v>
+      </c>
+      <c r="C53" s="24">
+        <f t="shared" si="3"/>
+        <v>47</v>
+      </c>
+      <c r="D53" s="20">
         <f t="shared" si="4"/>
-        <v>45474</v>
-      </c>
-      <c r="E26" s="27">
+        <v>46296</v>
+      </c>
+      <c r="E53" s="27">
+        <f t="shared" si="0"/>
+        <v>0.78333333333333333</v>
+      </c>
+      <c r="F53" s="27">
+        <f t="shared" si="5"/>
+        <v>685.41666666666663</v>
+      </c>
+      <c r="G53" s="27">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.77130715118020754</v>
+      </c>
+      <c r="H53" s="27">
+        <f t="shared" ca="1" si="2"/>
+        <v>674.89375728268158</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A54" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B54" s="26" t="s">
+        <v>12</v>
+      </c>
+      <c r="C54" s="24">
+        <f t="shared" si="3"/>
+        <v>48</v>
+      </c>
+      <c r="D54" s="20">
+        <f t="shared" si="4"/>
+        <v>46327</v>
+      </c>
+      <c r="E54" s="27">
+        <f t="shared" si="0"/>
+        <v>0.8</v>
+      </c>
+      <c r="F54" s="27">
+        <f t="shared" si="5"/>
+        <v>700</v>
+      </c>
+      <c r="G54" s="27">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.71234225328647338</v>
+      </c>
+      <c r="H54" s="27">
+        <f t="shared" ca="1" si="2"/>
+        <v>623.29947162566418</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A55" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B55" s="26" t="s">
+        <v>12</v>
+      </c>
+      <c r="C55" s="24">
+        <f t="shared" si="3"/>
+        <v>49</v>
+      </c>
+      <c r="D55" s="20">
+        <f t="shared" si="4"/>
+        <v>46357</v>
+      </c>
+      <c r="E55" s="27">
+        <f t="shared" si="0"/>
+        <v>0.81666666666666665</v>
+      </c>
+      <c r="F55" s="27">
+        <f t="shared" si="5"/>
+        <v>714.58333333333337</v>
+      </c>
+      <c r="G55" s="27">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.79107228292368514</v>
+      </c>
+      <c r="H55" s="27">
+        <f t="shared" ca="1" si="2"/>
+        <v>692.18824755822448</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A56" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B56" s="26" t="s">
+        <v>12</v>
+      </c>
+      <c r="C56" s="24">
+        <f t="shared" si="3"/>
+        <v>50</v>
+      </c>
+      <c r="D56" s="20">
+        <f t="shared" si="4"/>
+        <v>46388</v>
+      </c>
+      <c r="E56" s="27">
         <f t="shared" si="0"/>
         <v>0.83333333333333337</v>
       </c>
-      <c r="F26" s="27">
-        <f t="shared" si="1"/>
-        <v>160</v>
-      </c>
-      <c r="G26" s="27"/>
-      <c r="H26" s="27"/>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A27" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="B27" s="26" t="s">
-        <v>12</v>
-      </c>
-      <c r="C27" s="24">
-        <f t="shared" si="2"/>
-        <v>21</v>
-      </c>
-      <c r="D27" s="20">
+      <c r="F56" s="27">
+        <f t="shared" si="5"/>
+        <v>729.16666666666674</v>
+      </c>
+      <c r="G56" s="27">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.81627690658189489</v>
+      </c>
+      <c r="H56" s="27">
+        <f t="shared" ca="1" si="2"/>
+        <v>714.24229325915803</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A57" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B57" s="26" t="s">
+        <v>12</v>
+      </c>
+      <c r="C57" s="24">
+        <f t="shared" si="3"/>
+        <v>51</v>
+      </c>
+      <c r="D57" s="20">
         <f t="shared" si="4"/>
-        <v>45505</v>
-      </c>
-      <c r="E27" s="27">
+        <v>46419</v>
+      </c>
+      <c r="E57" s="27">
         <f t="shared" si="0"/>
-        <v>0.875</v>
-      </c>
-      <c r="F27" s="27">
-        <f t="shared" si="1"/>
-        <v>168</v>
-      </c>
-      <c r="G27" s="27"/>
-      <c r="H27" s="27"/>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A28" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="B28" s="26" t="s">
-        <v>12</v>
-      </c>
-      <c r="C28" s="24">
-        <f t="shared" si="2"/>
-        <v>22</v>
-      </c>
-      <c r="D28" s="20">
+        <v>0.85</v>
+      </c>
+      <c r="F57" s="27">
+        <f t="shared" si="5"/>
+        <v>743.75</v>
+      </c>
+      <c r="G57" s="27">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.88722716420532044</v>
+      </c>
+      <c r="H57" s="27">
+        <f t="shared" ca="1" si="2"/>
+        <v>776.32376867965536</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A58" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B58" s="26" t="s">
+        <v>12</v>
+      </c>
+      <c r="C58" s="24">
+        <f t="shared" si="3"/>
+        <v>52</v>
+      </c>
+      <c r="D58" s="20">
         <f t="shared" si="4"/>
-        <v>45536</v>
-      </c>
-      <c r="E28" s="27">
+        <v>46447</v>
+      </c>
+      <c r="E58" s="27">
+        <f t="shared" si="0"/>
+        <v>0.8666666666666667</v>
+      </c>
+      <c r="F58" s="27">
+        <f t="shared" si="5"/>
+        <v>758.33333333333337</v>
+      </c>
+      <c r="G58" s="27">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.85993266052557271</v>
+      </c>
+      <c r="H58" s="27">
+        <f t="shared" ca="1" si="2"/>
+        <v>752.44107795987611</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A59" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B59" s="26" t="s">
+        <v>12</v>
+      </c>
+      <c r="C59" s="24">
+        <f t="shared" si="3"/>
+        <v>53</v>
+      </c>
+      <c r="D59" s="20">
+        <f t="shared" si="4"/>
+        <v>46478</v>
+      </c>
+      <c r="E59" s="27">
+        <f t="shared" si="0"/>
+        <v>0.8833333333333333</v>
+      </c>
+      <c r="F59" s="27">
+        <f t="shared" si="5"/>
+        <v>772.91666666666663</v>
+      </c>
+      <c r="G59" s="27">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.92301435426997114</v>
+      </c>
+      <c r="H59" s="27">
+        <f t="shared" ca="1" si="2"/>
+        <v>807.6375599862248</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A60" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B60" s="26" t="s">
+        <v>12</v>
+      </c>
+      <c r="C60" s="24">
+        <f t="shared" si="3"/>
+        <v>54</v>
+      </c>
+      <c r="D60" s="20">
+        <f t="shared" si="4"/>
+        <v>46508</v>
+      </c>
+      <c r="E60" s="27">
+        <f t="shared" si="0"/>
+        <v>0.9</v>
+      </c>
+      <c r="F60" s="27">
+        <f t="shared" si="5"/>
+        <v>787.5</v>
+      </c>
+      <c r="G60" s="27">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.91889349694767641</v>
+      </c>
+      <c r="H60" s="27">
+        <f t="shared" ca="1" si="2"/>
+        <v>804.03180982921685</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A61" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B61" s="26" t="s">
+        <v>12</v>
+      </c>
+      <c r="C61" s="24">
+        <f t="shared" si="3"/>
+        <v>55</v>
+      </c>
+      <c r="D61" s="20">
+        <f t="shared" si="4"/>
+        <v>46539</v>
+      </c>
+      <c r="E61" s="27">
         <f t="shared" si="0"/>
         <v>0.91666666666666663</v>
       </c>
-      <c r="F28" s="27">
-        <f t="shared" si="1"/>
-        <v>176</v>
-      </c>
-      <c r="G28" s="27"/>
-      <c r="H28" s="27"/>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A29" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="B29" s="26" t="s">
-        <v>12</v>
-      </c>
-      <c r="C29" s="24">
-        <f t="shared" si="2"/>
-        <v>23</v>
-      </c>
-      <c r="D29" s="20">
+      <c r="F61" s="27">
+        <f t="shared" si="5"/>
+        <v>802.08333333333326</v>
+      </c>
+      <c r="G61" s="27">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.88723153964947632</v>
+      </c>
+      <c r="H61" s="27">
+        <f t="shared" ca="1" si="2"/>
+        <v>776.32759719329181</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A62" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B62" s="26" t="s">
+        <v>12</v>
+      </c>
+      <c r="C62" s="24">
+        <f t="shared" si="3"/>
+        <v>56</v>
+      </c>
+      <c r="D62" s="20">
         <f t="shared" si="4"/>
-        <v>45566</v>
-      </c>
-      <c r="E29" s="27">
+        <v>46569</v>
+      </c>
+      <c r="E62" s="27">
         <f t="shared" si="0"/>
-        <v>0.95833333333333337</v>
-      </c>
-      <c r="F29" s="27">
-        <f t="shared" si="1"/>
-        <v>184</v>
-      </c>
-      <c r="G29" s="27"/>
-      <c r="H29" s="27"/>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A30" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="B30" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="C30" s="14">
-        <f>C29+1</f>
-        <v>24</v>
-      </c>
-      <c r="D30" s="21">
-        <f>EDATE($D$7,C30)</f>
-        <v>45597</v>
-      </c>
-      <c r="E30" s="15">
-        <f>C30/24</f>
+        <v>0.93333333333333335</v>
+      </c>
+      <c r="F62" s="27">
+        <f t="shared" si="5"/>
+        <v>816.66666666666663</v>
+      </c>
+      <c r="G62" s="27">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.93649298172232753</v>
+      </c>
+      <c r="H62" s="27">
+        <f t="shared" ca="1" si="2"/>
+        <v>819.43135900703658</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A63" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B63" s="26" t="s">
+        <v>12</v>
+      </c>
+      <c r="C63" s="24">
+        <f t="shared" si="3"/>
+        <v>57</v>
+      </c>
+      <c r="D63" s="20">
+        <f t="shared" si="4"/>
+        <v>46600</v>
+      </c>
+      <c r="E63" s="27">
+        <f t="shared" si="0"/>
+        <v>0.95</v>
+      </c>
+      <c r="F63" s="27">
+        <f t="shared" si="5"/>
+        <v>831.25</v>
+      </c>
+      <c r="G63" s="27">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.91947715229476501</v>
+      </c>
+      <c r="H63" s="27">
+        <f t="shared" ca="1" si="2"/>
+        <v>804.54250825791939</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A64" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B64" s="26" t="s">
+        <v>12</v>
+      </c>
+      <c r="C64" s="24">
+        <f t="shared" si="3"/>
+        <v>58</v>
+      </c>
+      <c r="D64" s="20">
+        <f t="shared" si="4"/>
+        <v>46631</v>
+      </c>
+      <c r="E64" s="27">
+        <f t="shared" si="0"/>
+        <v>0.96666666666666667</v>
+      </c>
+      <c r="F64" s="27">
+        <f t="shared" si="5"/>
+        <v>845.83333333333337</v>
+      </c>
+      <c r="G64" s="27">
+        <f ca="1">NORMINV(RAND(), E64, 2*1/60)</f>
+        <v>0.94264231446100177</v>
+      </c>
+      <c r="H64" s="27">
+        <f t="shared" ca="1" si="2"/>
+        <v>824.81202515337657</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A65" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B65" s="26" t="s">
+        <v>12</v>
+      </c>
+      <c r="C65" s="24">
+        <f t="shared" si="3"/>
+        <v>59</v>
+      </c>
+      <c r="D65" s="20">
+        <f t="shared" si="4"/>
+        <v>46661</v>
+      </c>
+      <c r="E65" s="27">
+        <f t="shared" si="0"/>
+        <v>0.98333333333333328</v>
+      </c>
+      <c r="F65" s="27">
+        <f t="shared" si="5"/>
+        <v>860.41666666666663</v>
+      </c>
+      <c r="G65" s="27">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.94539309759991152</v>
+      </c>
+      <c r="H65" s="27">
+        <f t="shared" ca="1" si="2"/>
+        <v>827.21896039992259</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A66" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B66" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="C66" s="14">
+        <f>C65+1</f>
+        <v>60</v>
+      </c>
+      <c r="D66" s="21">
+        <f>EDATE($D$7,C66)</f>
+        <v>46692</v>
+      </c>
+      <c r="E66" s="15">
+        <f>C66/60</f>
         <v>1</v>
       </c>
-      <c r="F30" s="15">
-        <f>E30*192</f>
-        <v>192</v>
-      </c>
-      <c r="G30" s="15"/>
-      <c r="H30" s="15"/>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A31" s="5"/>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A33" t="s">
+      <c r="F66" s="15">
+        <f t="shared" si="5"/>
+        <v>875</v>
+      </c>
+      <c r="G66" s="15">
+        <f ca="1">NORMINV(RAND(), E66, 2*1/60)</f>
+        <v>0.99438873881364409</v>
+      </c>
+      <c r="H66" s="15">
+        <f t="shared" ca="1" si="2"/>
+        <v>870.09014646193862</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A67" s="5"/>
+    </row>
+    <row r="69" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A69" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A34" s="16">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A70" s="16">
         <v>44733</v>
       </c>
-      <c r="B34" t="s">
+      <c r="B70" t="s">
         <v>14</v>
       </c>
     </row>

</xml_diff>